<commit_message>
Adding support for Adventures. Moving CardLookup logic into a ViewModel for easier modification. Specific cards are labled in the output like the Bane.
</commit_message>
<xml_diff>
--- a/Data/Cards/DominionPickerData.xlsx
+++ b/Data/Cards/DominionPickerData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\VSO\Veleek\Dominion Picker\Data\Cards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\vso\Veleek\Dominion Picker\data\cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2694" uniqueCount="2089">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2944" uniqueCount="2178">
   <si>
     <t>Cellar</t>
   </si>
@@ -6287,6 +6287,273 @@
   </si>
   <si>
     <t>+1 Action\nReveal the top 3 cards of your deck.  The player to your left chooses one of them.  Discard that card.  Put the other cards into your hand.</t>
+  </si>
+  <si>
+    <t>Amulet</t>
+  </si>
+  <si>
+    <t>Artificer</t>
+  </si>
+  <si>
+    <t>Bridge Troll</t>
+  </si>
+  <si>
+    <t>Caravan Guard</t>
+  </si>
+  <si>
+    <t>Coin of the Realm</t>
+  </si>
+  <si>
+    <t>Distant Lands</t>
+  </si>
+  <si>
+    <t>Dungeon</t>
+  </si>
+  <si>
+    <t>Duplicate</t>
+  </si>
+  <si>
+    <t>Gear</t>
+  </si>
+  <si>
+    <t>Giant</t>
+  </si>
+  <si>
+    <t>Haunted Woods</t>
+  </si>
+  <si>
+    <t>Hireling</t>
+  </si>
+  <si>
+    <t>Lost City</t>
+  </si>
+  <si>
+    <t>Magpie</t>
+  </si>
+  <si>
+    <t>Messenger</t>
+  </si>
+  <si>
+    <t>Miser</t>
+  </si>
+  <si>
+    <t>Page</t>
+  </si>
+  <si>
+    <t>Peasant</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>Ranger</t>
+  </si>
+  <si>
+    <t>Ratcatcher</t>
+  </si>
+  <si>
+    <t>Relic</t>
+  </si>
+  <si>
+    <t>Royal Carriage</t>
+  </si>
+  <si>
+    <t>Storyteller</t>
+  </si>
+  <si>
+    <t>Swamp Hag</t>
+  </si>
+  <si>
+    <t>Treasure Trove</t>
+  </si>
+  <si>
+    <t>Alms</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>Ball</t>
+  </si>
+  <si>
+    <t>Bonfire</t>
+  </si>
+  <si>
+    <t>Borrow</t>
+  </si>
+  <si>
+    <t>Champion</t>
+  </si>
+  <si>
+    <t>Disciple</t>
+  </si>
+  <si>
+    <t>Action Traveller</t>
+  </si>
+  <si>
+    <t>Expedition</t>
+  </si>
+  <si>
+    <t>Ferry</t>
+  </si>
+  <si>
+    <t>Fugitive</t>
+  </si>
+  <si>
+    <t>Hero</t>
+  </si>
+  <si>
+    <t>Inheritance</t>
+  </si>
+  <si>
+    <t>Lost Arts</t>
+  </si>
+  <si>
+    <t>Mission</t>
+  </si>
+  <si>
+    <t>Pathfinding</t>
+  </si>
+  <si>
+    <t>Pilgrimage</t>
+  </si>
+  <si>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>Quest</t>
+  </si>
+  <si>
+    <t>Raid</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>Scouting Party</t>
+  </si>
+  <si>
+    <t>Seaway</t>
+  </si>
+  <si>
+    <t>Soldier</t>
+  </si>
+  <si>
+    <t>Action Attack Traveller</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>Action Reserve</t>
+  </si>
+  <si>
+    <t>Trade</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Travelling Fair</t>
+  </si>
+  <si>
+    <t>Treasure Hunter</t>
+  </si>
+  <si>
+    <t>Warrior</t>
+  </si>
+  <si>
+    <t>Wine Merchant</t>
+  </si>
+  <si>
+    <t>Adventures</t>
+  </si>
+  <si>
+    <t>Action Attack Duration</t>
+  </si>
+  <si>
+    <t>Action Duration Reaction</t>
+  </si>
+  <si>
+    <t>Treasure Reserve</t>
+  </si>
+  <si>
+    <t>Action Reserve Victory</t>
+  </si>
+  <si>
+    <t>Treasure Attack</t>
+  </si>
+  <si>
+    <t>Once per turn: If you have no Treasures in play, gain a card costing up to $4.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Take your -Coin1.png token. Gain 2 cards each costing up to Coin4.png.</t>
+  </si>
+  <si>
+    <t>Trash up to 2 cards you have in play.</t>
+  </si>
+  <si>
+    <t>Put this on your Tavern mat.\nWorth 4 VP.png if on your Tavern mat at the end of the game (otherwise worth 0 VP.png).</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Draw 2 extra cards for your next hand.</t>
+  </si>
+  <si>
+    <t>Guide</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Raze</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Transmogrify</t>
+  </si>
+  <si>
+    <t>Now and at the start of your next turn, choose one: +Coin1.png; or trash a card from your hand; or gain a Silver.</t>
+  </si>
+  <si>
+    <t>+1 Action\n+1 Card\n+Coin1.png\nDiscard any number of cards. You may gain a card costing exactly Coin1.png per card discarded, putting it on top of your deck.</t>
+  </si>
+  <si>
+    <t>+1 Buy\nOnce per turn: If your -1 Card token isn't on your deck, put it there and +Coin1.png.</t>
+  </si>
+  <si>
+    <t>Each other player takes his -Coin1.png token. Now and at the start of your next turn:\n+1 Buy\n_____\nWhile this is in play, cards cost Coin1.png less on your turns, but not less than Coin0.png.</t>
+  </si>
+  <si>
+    <t>+1 Card\n+1 Action\nAt the start of your next turn, +Coin1.png\nWhen another player plays an Attack card, you may play this from your hand. (+1 Action has no effect if it's not your turn.)</t>
+  </si>
+  <si>
+    <t>+1 Action\nFor the rest of the game, when another player plays an Attack, it doesn't affect you, and when you play an Action, +1 Action.\n(This stays in play. This is not in the Supply.)</t>
+  </si>
+  <si>
+    <t>Coin1.png\nWhen you play this, put it on your Tavern mat.\nDirectly after resolving an Action, you may call this, for +2 Actions.</t>
+  </si>
+  <si>
+    <t>You may play an Action card from your hand twice. Gain a copy of it.\nWhen you discard this from play, you may exchange it for a Teacher.\n(This is not in the Supply)</t>
+  </si>
+  <si>
+    <t>+1 Action\nNow and at the start of your next turn: +2 Cards, then discard 2 cards.</t>
+  </si>
+  <si>
+    <t>Put this on your Tavern mat.\n_____\nWhen you gain a card costing up to Coin6.png, you may call this, to gain a copy of that card.</t>
+  </si>
+  <si>
+    <t>Move your -Coin2.png cost token to an Action Supply pile (cards from that pile cost Coin2.png less on your turns, but not less than Coin0.png.</t>
+  </si>
+  <si>
+    <t>+2 Cards\n+1 Action\nDiscard a card.\n_____\nWhen you discard this from play, you may exchange it for a Disciple.\n(This is not in the Supply)</t>
   </si>
 </sst>
 </file>
@@ -6787,7 +7054,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -6808,6 +7075,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -6921,8 +7190,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:V245" totalsRowShown="0">
-  <autoFilter ref="A1:V245"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:V303" totalsRowShown="0">
+  <autoFilter ref="A1:V303"/>
   <tableColumns count="22">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Name"/>
@@ -7215,13 +7484,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:V245"/>
+  <dimension ref="A1:V303"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C190" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C245" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F225" sqref="F225"/>
+      <selection pane="bottomRight" activeCell="H261" sqref="H261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15551,10 +15820,1051 @@
         <v>608</v>
       </c>
     </row>
+    <row r="246" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>245</v>
+      </c>
+      <c r="B246" t="s">
+        <v>2115</v>
+      </c>
+      <c r="C246" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D246" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E246" s="10" t="s">
+        <v>598</v>
+      </c>
+      <c r="F246" s="11" t="s">
+        <v>2154</v>
+      </c>
+      <c r="G246" s="1" t="s">
+        <v>2155</v>
+      </c>
+    </row>
+    <row r="247" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>246</v>
+      </c>
+      <c r="B247" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C247" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D247" t="s">
+        <v>112</v>
+      </c>
+      <c r="E247" s="10" t="s">
+        <v>599</v>
+      </c>
+      <c r="F247" s="5" t="s">
+        <v>2166</v>
+      </c>
+    </row>
+    <row r="248" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>247</v>
+      </c>
+      <c r="B248" t="s">
+        <v>2090</v>
+      </c>
+      <c r="C248" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D248" t="s">
+        <v>2</v>
+      </c>
+      <c r="E248" s="10" t="s">
+        <v>602</v>
+      </c>
+      <c r="F248" s="5" t="s">
+        <v>2167</v>
+      </c>
+    </row>
+    <row r="249" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>248</v>
+      </c>
+      <c r="B249" t="s">
+        <v>2117</v>
+      </c>
+      <c r="C249" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D249" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E249" s="10" t="s">
+        <v>602</v>
+      </c>
+      <c r="F249" s="5" t="s">
+        <v>2156</v>
+      </c>
+    </row>
+    <row r="250" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>249</v>
+      </c>
+      <c r="B250" t="s">
+        <v>2118</v>
+      </c>
+      <c r="C250" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D250" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E250" s="10" t="s">
+        <v>599</v>
+      </c>
+      <c r="F250" s="5" t="s">
+        <v>2157</v>
+      </c>
+    </row>
+    <row r="251" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>250</v>
+      </c>
+      <c r="B251" t="s">
+        <v>2119</v>
+      </c>
+      <c r="C251" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D251" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E251" s="10" t="s">
+        <v>598</v>
+      </c>
+      <c r="F251" s="5" t="s">
+        <v>2168</v>
+      </c>
+    </row>
+    <row r="252" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>251</v>
+      </c>
+      <c r="B252" t="s">
+        <v>2091</v>
+      </c>
+      <c r="C252" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D252" t="s">
+        <v>2149</v>
+      </c>
+      <c r="E252" s="10" t="s">
+        <v>602</v>
+      </c>
+      <c r="F252" s="5" t="s">
+        <v>2169</v>
+      </c>
+    </row>
+    <row r="253" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>252</v>
+      </c>
+      <c r="B253" t="s">
+        <v>2092</v>
+      </c>
+      <c r="C253" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D253" t="s">
+        <v>2150</v>
+      </c>
+      <c r="E253" s="10" t="s">
+        <v>599</v>
+      </c>
+      <c r="F253" s="5" t="s">
+        <v>2170</v>
+      </c>
+    </row>
+    <row r="254" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>253</v>
+      </c>
+      <c r="B254" t="s">
+        <v>2120</v>
+      </c>
+      <c r="C254" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D254" t="s">
+        <v>112</v>
+      </c>
+      <c r="E254" s="10" t="s">
+        <v>600</v>
+      </c>
+      <c r="F254" s="5" t="s">
+        <v>2171</v>
+      </c>
+    </row>
+    <row r="255" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>254</v>
+      </c>
+      <c r="B255" t="s">
+        <v>2093</v>
+      </c>
+      <c r="C255" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D255" t="s">
+        <v>2151</v>
+      </c>
+      <c r="E255" s="10" t="s">
+        <v>601</v>
+      </c>
+      <c r="F255" s="5" t="s">
+        <v>2172</v>
+      </c>
+    </row>
+    <row r="256" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>255</v>
+      </c>
+      <c r="B256" t="s">
+        <v>2121</v>
+      </c>
+      <c r="C256" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D256" t="s">
+        <v>2122</v>
+      </c>
+      <c r="E256" s="10" t="s">
+        <v>602</v>
+      </c>
+      <c r="F256" s="5" t="s">
+        <v>2173</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>256</v>
+      </c>
+      <c r="B257" t="s">
+        <v>2094</v>
+      </c>
+      <c r="C257" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D257" t="s">
+        <v>2152</v>
+      </c>
+      <c r="E257" s="10" t="s">
+        <v>602</v>
+      </c>
+      <c r="F257" s="5" t="s">
+        <v>2158</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>257</v>
+      </c>
+      <c r="B258" t="s">
+        <v>2095</v>
+      </c>
+      <c r="C258" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D258" t="s">
+        <v>112</v>
+      </c>
+      <c r="E258" s="10" t="s">
+        <v>599</v>
+      </c>
+      <c r="F258" s="5" t="s">
+        <v>2174</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>258</v>
+      </c>
+      <c r="B259" t="s">
+        <v>2096</v>
+      </c>
+      <c r="C259" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D259" t="s">
+        <v>2141</v>
+      </c>
+      <c r="E259" s="10" t="s">
+        <v>2159</v>
+      </c>
+      <c r="F259" s="5" t="s">
+        <v>2175</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>259</v>
+      </c>
+      <c r="B260" t="s">
+        <v>2123</v>
+      </c>
+      <c r="C260" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D260" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E260" s="10" t="s">
+        <v>599</v>
+      </c>
+      <c r="F260" s="5" t="s">
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>260</v>
+      </c>
+      <c r="B261" t="s">
+        <v>2124</v>
+      </c>
+      <c r="C261" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D261" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E261" s="10" t="s">
+        <v>599</v>
+      </c>
+      <c r="F261" s="5" t="s">
+        <v>2176</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>261</v>
+      </c>
+      <c r="B262" t="s">
+        <v>2125</v>
+      </c>
+      <c r="C262" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D262" t="s">
+        <v>2122</v>
+      </c>
+      <c r="E262" s="10" t="s">
+        <v>2159</v>
+      </c>
+      <c r="F262" s="5" t="s">
+        <v>2177</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>262</v>
+      </c>
+      <c r="B263" t="s">
+        <v>2097</v>
+      </c>
+      <c r="C263" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D263" t="s">
+        <v>112</v>
+      </c>
+      <c r="E263" s="10" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>263</v>
+      </c>
+      <c r="B264" t="s">
+        <v>2098</v>
+      </c>
+      <c r="C264" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D264" t="s">
+        <v>18</v>
+      </c>
+      <c r="E264" s="10" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>264</v>
+      </c>
+      <c r="B265" t="s">
+        <v>2161</v>
+      </c>
+      <c r="C265" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D265" t="s">
+        <v>2141</v>
+      </c>
+      <c r="E265" s="10" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>265</v>
+      </c>
+      <c r="B266" t="s">
+        <v>2099</v>
+      </c>
+      <c r="C266" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D266" t="s">
+        <v>2149</v>
+      </c>
+      <c r="E266" s="10" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>266</v>
+      </c>
+      <c r="B267" t="s">
+        <v>2126</v>
+      </c>
+      <c r="C267" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D267" t="s">
+        <v>2122</v>
+      </c>
+      <c r="E267" s="10" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>267</v>
+      </c>
+      <c r="B268" t="s">
+        <v>2100</v>
+      </c>
+      <c r="C268" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D268" t="s">
+        <v>112</v>
+      </c>
+      <c r="E268" s="10" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A269">
+        <v>268</v>
+      </c>
+      <c r="B269" t="s">
+        <v>2127</v>
+      </c>
+      <c r="C269" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D269" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E269" s="10" t="s">
+        <v>2162</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A270">
+        <v>269</v>
+      </c>
+      <c r="B270" t="s">
+        <v>2128</v>
+      </c>
+      <c r="C270" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D270" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E270" s="10" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A271">
+        <v>270</v>
+      </c>
+      <c r="B271" t="s">
+        <v>2101</v>
+      </c>
+      <c r="C271" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D271" t="s">
+        <v>2</v>
+      </c>
+      <c r="E271" s="10" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>271</v>
+      </c>
+      <c r="B272" t="s">
+        <v>2102</v>
+      </c>
+      <c r="C272" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D272" t="s">
+        <v>2</v>
+      </c>
+      <c r="E272" s="10" t="s">
+        <v>2159</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A273">
+        <v>272</v>
+      </c>
+      <c r="B273" t="s">
+        <v>2103</v>
+      </c>
+      <c r="C273" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D273" t="s">
+        <v>2</v>
+      </c>
+      <c r="E273" s="10" t="s">
+        <v>2159</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A274">
+        <v>273</v>
+      </c>
+      <c r="B274" t="s">
+        <v>2104</v>
+      </c>
+      <c r="C274" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D274" t="s">
+        <v>2</v>
+      </c>
+      <c r="E274" s="10" t="s">
+        <v>2159</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A275">
+        <v>274</v>
+      </c>
+      <c r="B275" t="s">
+        <v>2129</v>
+      </c>
+      <c r="C275" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D275" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E275" s="10" t="s">
+        <v>2159</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>275</v>
+      </c>
+      <c r="B276" t="s">
+        <v>2105</v>
+      </c>
+      <c r="C276" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D276" t="s">
+        <v>2122</v>
+      </c>
+      <c r="E276" s="10" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A277">
+        <v>276</v>
+      </c>
+      <c r="B277" t="s">
+        <v>2130</v>
+      </c>
+      <c r="C277" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D277" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E277" s="10" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A278">
+        <v>277</v>
+      </c>
+      <c r="B278" t="s">
+        <v>2106</v>
+      </c>
+      <c r="C278" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D278" t="s">
+        <v>2122</v>
+      </c>
+      <c r="E278" s="10" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A279">
+        <v>278</v>
+      </c>
+      <c r="B279" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C279" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D279" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E279" s="10" t="s">
+        <v>2159</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A280">
+        <v>279</v>
+      </c>
+      <c r="B280" t="s">
+        <v>2132</v>
+      </c>
+      <c r="C280" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D280" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E280" s="10" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A281">
+        <v>280</v>
+      </c>
+      <c r="B281" t="s">
+        <v>2107</v>
+      </c>
+      <c r="C281" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D281" t="s">
+        <v>2</v>
+      </c>
+      <c r="E281" s="10" t="s">
+        <v>2159</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A282">
+        <v>281</v>
+      </c>
+      <c r="B282" t="s">
+        <v>2133</v>
+      </c>
+      <c r="C282" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D282" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E282" s="10" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A283">
+        <v>282</v>
+      </c>
+      <c r="B283" t="s">
+        <v>2134</v>
+      </c>
+      <c r="C283" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D283" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E283" s="10" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A284">
+        <v>283</v>
+      </c>
+      <c r="B284" t="s">
+        <v>2108</v>
+      </c>
+      <c r="C284" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D284" t="s">
+        <v>2</v>
+      </c>
+      <c r="E284" s="10" t="s">
+        <v>2159</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A285">
+        <v>284</v>
+      </c>
+      <c r="B285" t="s">
+        <v>2109</v>
+      </c>
+      <c r="C285" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D285" t="s">
+        <v>2141</v>
+      </c>
+      <c r="E285" s="10" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A286">
+        <v>285</v>
+      </c>
+      <c r="B286" t="s">
+        <v>2163</v>
+      </c>
+      <c r="C286" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D286" t="s">
+        <v>2</v>
+      </c>
+      <c r="E286" s="10" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>286</v>
+      </c>
+      <c r="B287" t="s">
+        <v>2110</v>
+      </c>
+      <c r="C287" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D287" t="s">
+        <v>2153</v>
+      </c>
+      <c r="E287" s="10" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A288">
+        <v>287</v>
+      </c>
+      <c r="B288" t="s">
+        <v>2111</v>
+      </c>
+      <c r="C288" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D288" t="s">
+        <v>2141</v>
+      </c>
+      <c r="E288" s="10" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>288</v>
+      </c>
+      <c r="B289" t="s">
+        <v>2135</v>
+      </c>
+      <c r="C289" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D289" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E289" s="10" t="s">
+        <v>2164</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>289</v>
+      </c>
+      <c r="B290" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C290" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D290" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E290" s="10" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>290</v>
+      </c>
+      <c r="B291" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C291" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D291" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E291" s="10" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A292">
+        <v>291</v>
+      </c>
+      <c r="B292" t="s">
+        <v>2138</v>
+      </c>
+      <c r="C292" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D292" t="s">
+        <v>2139</v>
+      </c>
+      <c r="E292" s="10" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>292</v>
+      </c>
+      <c r="B293" t="s">
+        <v>2112</v>
+      </c>
+      <c r="C293" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D293" t="s">
+        <v>2</v>
+      </c>
+      <c r="E293" s="10" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A294">
+        <v>293</v>
+      </c>
+      <c r="B294" t="s">
+        <v>2113</v>
+      </c>
+      <c r="C294" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D294" t="s">
+        <v>2149</v>
+      </c>
+      <c r="E294" s="10" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>294</v>
+      </c>
+      <c r="B295" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C295" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D295" t="s">
+        <v>2141</v>
+      </c>
+      <c r="E295" s="10" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>295</v>
+      </c>
+      <c r="B296" t="s">
+        <v>2142</v>
+      </c>
+      <c r="C296" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D296" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E296" s="10" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>296</v>
+      </c>
+      <c r="B297" t="s">
+        <v>2143</v>
+      </c>
+      <c r="C297" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D297" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E297" s="10" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>297</v>
+      </c>
+      <c r="B298" t="s">
+        <v>2165</v>
+      </c>
+      <c r="C298" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D298" t="s">
+        <v>2141</v>
+      </c>
+      <c r="E298" s="10" t="s">
+        <v>2159</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A299">
+        <v>298</v>
+      </c>
+      <c r="B299" t="s">
+        <v>2144</v>
+      </c>
+      <c r="C299" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D299" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E299" s="10" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>299</v>
+      </c>
+      <c r="B300" t="s">
+        <v>2145</v>
+      </c>
+      <c r="C300" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D300" t="s">
+        <v>2122</v>
+      </c>
+      <c r="E300" s="10" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A301">
+        <v>300</v>
+      </c>
+      <c r="B301" t="s">
+        <v>2114</v>
+      </c>
+      <c r="C301" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D301" t="s">
+        <v>182</v>
+      </c>
+      <c r="E301" s="10" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A302">
+        <v>301</v>
+      </c>
+      <c r="B302" t="s">
+        <v>2146</v>
+      </c>
+      <c r="C302" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D302" t="s">
+        <v>2139</v>
+      </c>
+      <c r="E302" s="10" t="s">
+        <v>2159</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A303">
+        <v>302</v>
+      </c>
+      <c r="B303" t="s">
+        <v>2147</v>
+      </c>
+      <c r="C303" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D303" t="s">
+        <v>2141</v>
+      </c>
+      <c r="E303" s="10" t="s">
+        <v>602</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Adding all data for Adventures Cards. Cleaning up some other localized strings.
</commit_message>
<xml_diff>
--- a/Data/Cards/DominionPickerData.xlsx
+++ b/Data/Cards/DominionPickerData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\vso\Veleek\Dominion Picker\data\cards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\VSO\Veleek\Dominion Picker\Data\Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2944" uniqueCount="2178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2985" uniqueCount="2219">
   <si>
     <t>Cellar</t>
   </si>
@@ -6490,15 +6490,9 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Take your -Coin1.png token. Gain 2 cards each costing up to Coin4.png.</t>
-  </si>
-  <si>
     <t>Trash up to 2 cards you have in play.</t>
   </si>
   <si>
-    <t>Put this on your Tavern mat.\nWorth 4 VP.png if on your Tavern mat at the end of the game (otherwise worth 0 VP.png).</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
@@ -6520,40 +6514,169 @@
     <t>Transmogrify</t>
   </si>
   <si>
-    <t>Now and at the start of your next turn, choose one: +Coin1.png; or trash a card from your hand; or gain a Silver.</t>
-  </si>
-  <si>
-    <t>+1 Action\n+1 Card\n+Coin1.png\nDiscard any number of cards. You may gain a card costing exactly Coin1.png per card discarded, putting it on top of your deck.</t>
-  </si>
-  <si>
-    <t>+1 Buy\nOnce per turn: If your -1 Card token isn't on your deck, put it there and +Coin1.png.</t>
-  </si>
-  <si>
-    <t>Each other player takes his -Coin1.png token. Now and at the start of your next turn:\n+1 Buy\n_____\nWhile this is in play, cards cost Coin1.png less on your turns, but not less than Coin0.png.</t>
-  </si>
-  <si>
-    <t>+1 Card\n+1 Action\nAt the start of your next turn, +Coin1.png\nWhen another player plays an Attack card, you may play this from your hand. (+1 Action has no effect if it's not your turn.)</t>
-  </si>
-  <si>
     <t>+1 Action\nFor the rest of the game, when another player plays an Attack, it doesn't affect you, and when you play an Action, +1 Action.\n(This stays in play. This is not in the Supply.)</t>
   </si>
   <si>
-    <t>Coin1.png\nWhen you play this, put it on your Tavern mat.\nDirectly after resolving an Action, you may call this, for +2 Actions.</t>
-  </si>
-  <si>
     <t>You may play an Action card from your hand twice. Gain a copy of it.\nWhen you discard this from play, you may exchange it for a Teacher.\n(This is not in the Supply)</t>
   </si>
   <si>
     <t>+1 Action\nNow and at the start of your next turn: +2 Cards, then discard 2 cards.</t>
   </si>
   <si>
-    <t>Put this on your Tavern mat.\n_____\nWhen you gain a card costing up to Coin6.png, you may call this, to gain a copy of that card.</t>
-  </si>
-  <si>
-    <t>Move your -Coin2.png cost token to an Action Supply pile (cards from that pile cost Coin2.png less on your turns, but not less than Coin0.png.</t>
-  </si>
-  <si>
     <t>+2 Cards\n+1 Action\nDiscard a card.\n_____\nWhen you discard this from play, you may exchange it for a Disciple.\n(This is not in the Supply)</t>
+  </si>
+  <si>
+    <t>Now and at the start of your next turn, choose one: +$1; or trash a card from your hand; or gain a Silver.</t>
+  </si>
+  <si>
+    <t>+1 Action\n+1 Card\n+$1\nDiscard any number of cards. You may gain a card costing exactly $1 per card discarded, putting it on top of your deck.</t>
+  </si>
+  <si>
+    <t>Take your -$1 token. Gain 2 cards each costing up to $4.</t>
+  </si>
+  <si>
+    <t>+1 Buy\nOnce per turn: If your -1 Card token isn't on your deck, put it there and +$1.</t>
+  </si>
+  <si>
+    <t>Each other player takes his -$1 token. Now and at the start of your next turn:\n+1 Buy\n_____\nWhile this is in play, cards cost $1 less on your turns, but not less than $0.</t>
+  </si>
+  <si>
+    <t>+1 Card\n+1 Action\nAt the start of your next turn, +$1\nWhen another player plays an Attack card, you may play this from your hand. (+1 Action has no effect if it's not your turn.)</t>
+  </si>
+  <si>
+    <t>$1\nWhen you play this, put it on your Tavern mat.\nDirectly after resolving an Action, you may call this, for +2 Actions.</t>
+  </si>
+  <si>
+    <t>Put this on your Tavern mat.\nWorth 4 {VP} if on your Tavern mat at the end of the game (otherwise worth 0 {VP}).</t>
+  </si>
+  <si>
+    <t>Put this on your Tavern mat.\n_____\nWhen you gain a card costing up to $6, you may call this, to gain a copy of that card.</t>
+  </si>
+  <si>
+    <t>Move your -$2 cost token to an Action Supply pile (cards from that pile cost $2 less on your turns, but not less than $0.</t>
+  </si>
+  <si>
+    <t>+2 Cards\nSet aside up to 2 cards from your hand face down. At the start of your next turn, put them into your hand.</t>
+  </si>
+  <si>
+    <t>Turn your Journey token over (it starts face up). If it's face down, +$1. If it's face up, +$5, and each other player reveals the top card of his deck, trashes it if it costs from $3 to $6, and otherwise discards it and gains a Curse.</t>
+  </si>
+  <si>
+    <t>+1 Card\n+1 Action\nPut this on your Tavern mat.\n_____\nAt the start of your turn, you may call this, to discard your hand and draw 5 cards.</t>
+  </si>
+  <si>
+    <t>Until you next turn, when any other player buys a card, he puts his hand on top of his deck in any order.\nAt the start of your next turn:\n+3 Cards</t>
+  </si>
+  <si>
+    <t>+$2\nGain a Treasure.\n_____\nWhen you discard this from play, you may exchange it for a Champion.\n(This is not in the Supply)</t>
+  </si>
+  <si>
+    <t>At the start of each of your turns for the rest of the game:\n+1 Card\n(This stays in play)</t>
+  </si>
+  <si>
+    <t>Once per game: Set aside a non-Victory Action card from the Supply costing up to $4. Move your Estate token to it (your Estates gain the abilities and types of that card).</t>
+  </si>
+  <si>
+    <t>Move your +1 Action token to an Action Supply pile (when you play a card from that pile, you first get +1 Action).</t>
+  </si>
+  <si>
+    <t>+2 Cards\n+2 Actions\n_____\nWhen you gain this, each other player draws a card.</t>
+  </si>
+  <si>
+    <t>+1 Card\n+1 Action\nReveal the top card of your deck. If it's a Treasure, put it into your hand. If it's an Action or Victory card, gain a Magpie.</t>
+  </si>
+  <si>
+    <t>+1 Buy\n+$2\nYou may put your deck into your discard pile.\n_____\nWhen this is your first buy in a turn, gain a card costing up to $4, and each other player gains a copy of it.</t>
+  </si>
+  <si>
+    <t>Choose one: Put a Copper from your hand onto your Tavern mat; or +$1 per Copper on your Tavern mat.</t>
+  </si>
+  <si>
+    <t>Once per turn: If the previous turn wasn't yours, take another turn after this one, in which you can't buy cards.</t>
+  </si>
+  <si>
+    <t>+1 Card\n+1 Action\n_____\nWhen you discard this from play, you may exchange it for a Treasure Hunter</t>
+  </si>
+  <si>
+    <t>Move your +1 Card token to an Action Supply pile (when you play a card from that pile, you first get +1 Card).</t>
+  </si>
+  <si>
+    <t>+1 Buy\n+$1\n_____\nWhen you discard this from play, you may exchange it for a Soldier.</t>
+  </si>
+  <si>
+    <t>Once per turn: Turn your Journey token over (it starts face up); then if it's face up, choose up to 3 differently named cards you have in play and gain a copy of each.</t>
+  </si>
+  <si>
+    <t>Move your Trashing token to an Action Supply pile (when you buy a card from that pile, you may trash a card from your hand.)</t>
+  </si>
+  <si>
+    <t>+1 Card\n+2 Actions\n_____\nWhen you buy this, gain another Port.</t>
+  </si>
+  <si>
+    <t>You may discard an Attack, two Curses, or six cards. If you do, gain a Gold.</t>
+  </si>
+  <si>
+    <t>Gain a Silver per Silver you have in play. Each other player puts his -1 Card token on his deck.</t>
+  </si>
+  <si>
+    <t>+1 Buy\nTurn your Journey token over (it starts face up). If it's face up, +5 Cards.</t>
+  </si>
+  <si>
+    <t>+1 Card\n+1 Action\nPut this on your Tavern mat.\nAt the start of your turn, you may call this to trash a card from your hand.</t>
+  </si>
+  <si>
+    <t>+1 Action\nTrash this or a card from your hand. Look at a number of cards from the top of your deck equal to the cost in $_ of the trashed card. Put one into your hand and discard the rest.</t>
+  </si>
+  <si>
+    <t>$2\nWhen you play this, each other player puts his -1 Card token on his deck.</t>
+  </si>
+  <si>
+    <t>+1 Action\nPut this on your Tavern mat.\n_____\nDirectly after resolving an Action, if it's still in play, you may call this, to replay that Action.</t>
+  </si>
+  <si>
+    <t>+1 Buy\nOnce per turn: Set aside a card from your hand, and put it into your hand at end of turn (after drawing).</t>
+  </si>
+  <si>
+    <t>+1 Buy\nLook at the top 5 cards of your deck. Discard 3 of them and put the rest back on top of your deck in any order.</t>
+  </si>
+  <si>
+    <t>Gain an Action card costing up to $4. Move your +1 Buy token to its pile (when you play a card from that pile, you first get +1 Buy).</t>
+  </si>
+  <si>
+    <t>+$2\n+$1 per other Attack you have in play. Each other player with 4 or more cards in hand discards a card.\n_____\nWhen you discard this from play, you may exchange it for a Fugitive.\n(This is not in the Supply)</t>
+  </si>
+  <si>
+    <t>+1 Action\n+1 $1\nPlay up to 3 Treasures from your hand. Pay all of your $_; +1 Card per $_ paid.</t>
+  </si>
+  <si>
+    <t>Until your next turn, when any other player buys a card, he gains a Curse.\nAt the start of your next turn:\n+$3</t>
+  </si>
+  <si>
+    <t>Put this on your Tavern mat.\n_____\nAt the start of your turn, you may call this, to move your +1 Card, +1 Action, +1 Buy, or +$1 token to an Action Supply pile you have no token on (when you play a card from that pile you first get that bonus).\n(This is not in the Supply)</t>
+  </si>
+  <si>
+    <t>Trash up to 2 cards from your hand.\nGain a Silver per card you trashed.</t>
+  </si>
+  <si>
+    <t>Move your +$1 token to an Action Supply pile (when you play a card from that pile, you first get +$1).</t>
+  </si>
+  <si>
+    <t>+1 Action\nPut this on your Tavern mat.\n_____\nAt the start of your turn, you may call this, to trash a card from your hand, gain a card costing up to $1 more than it, and put that card into your hand.</t>
+  </si>
+  <si>
+    <t>+2 Buys\nWhen you gain a card this turn, you may put it on top of your deck.</t>
+  </si>
+  <si>
+    <t>+1 Action\n+$1\nGain a Silver per card the player to your right gained in his last turn.\n_____\nWhen you discard this from play, you may exchange it for a Warrior.\n(This is not in the Supply)</t>
+  </si>
+  <si>
+    <t>$2\nWhen you play this, gain a Gold and a Copper.</t>
+  </si>
+  <si>
+    <t>+2 Cards\nFor each Traveller you have in play (including this) each other player discards the top card of his deck and trashes it if it costs $3 or $4.\n_____\nWhen you discard this from play, you may exchange it for a Hero.\n(This is not in the Supply)</t>
+  </si>
+  <si>
+    <t>+1 Buy\n+$4\nPut this on your Tavern mat.\n_____\nAt the end of your Buy phase, if you have at least $2 unspent, you may discard this from your Tavern mat.</t>
   </si>
 </sst>
 </file>
@@ -7487,10 +7610,10 @@
   <dimension ref="A1:V303"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C245" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C240" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H261" sqref="H261"/>
+      <selection pane="bottomRight" activeCell="B246" sqref="B246:B303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7500,7 +7623,7 @@
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="249.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="15.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="39.42578125" style="5" customWidth="1"/>
     <col min="11" max="22" width="15.7109375" style="1" customWidth="1"/>
@@ -15860,7 +15983,7 @@
         <v>599</v>
       </c>
       <c r="F247" s="5" t="s">
-        <v>2166</v>
+        <v>2168</v>
       </c>
     </row>
     <row r="248" spans="1:15" x14ac:dyDescent="0.25">
@@ -15880,7 +16003,7 @@
         <v>602</v>
       </c>
       <c r="F248" s="5" t="s">
-        <v>2167</v>
+        <v>2169</v>
       </c>
     </row>
     <row r="249" spans="1:15" x14ac:dyDescent="0.25">
@@ -15900,7 +16023,7 @@
         <v>602</v>
       </c>
       <c r="F249" s="5" t="s">
-        <v>2156</v>
+        <v>2170</v>
       </c>
     </row>
     <row r="250" spans="1:15" x14ac:dyDescent="0.25">
@@ -15920,7 +16043,7 @@
         <v>599</v>
       </c>
       <c r="F250" s="5" t="s">
-        <v>2157</v>
+        <v>2156</v>
       </c>
     </row>
     <row r="251" spans="1:15" x14ac:dyDescent="0.25">
@@ -15940,7 +16063,7 @@
         <v>598</v>
       </c>
       <c r="F251" s="5" t="s">
-        <v>2168</v>
+        <v>2171</v>
       </c>
     </row>
     <row r="252" spans="1:15" x14ac:dyDescent="0.25">
@@ -15960,7 +16083,7 @@
         <v>602</v>
       </c>
       <c r="F252" s="5" t="s">
-        <v>2169</v>
+        <v>2172</v>
       </c>
     </row>
     <row r="253" spans="1:15" x14ac:dyDescent="0.25">
@@ -15980,7 +16103,7 @@
         <v>599</v>
       </c>
       <c r="F253" s="5" t="s">
-        <v>2170</v>
+        <v>2173</v>
       </c>
     </row>
     <row r="254" spans="1:15" x14ac:dyDescent="0.25">
@@ -16000,7 +16123,7 @@
         <v>600</v>
       </c>
       <c r="F254" s="5" t="s">
-        <v>2171</v>
+        <v>2164</v>
       </c>
     </row>
     <row r="255" spans="1:15" x14ac:dyDescent="0.25">
@@ -16020,7 +16143,7 @@
         <v>601</v>
       </c>
       <c r="F255" s="5" t="s">
-        <v>2172</v>
+        <v>2174</v>
       </c>
     </row>
     <row r="256" spans="1:15" x14ac:dyDescent="0.25">
@@ -16040,7 +16163,7 @@
         <v>602</v>
       </c>
       <c r="F256" s="5" t="s">
-        <v>2173</v>
+        <v>2165</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.25">
@@ -16060,7 +16183,7 @@
         <v>602</v>
       </c>
       <c r="F257" s="5" t="s">
-        <v>2158</v>
+        <v>2175</v>
       </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.25">
@@ -16080,7 +16203,7 @@
         <v>599</v>
       </c>
       <c r="F258" s="5" t="s">
-        <v>2174</v>
+        <v>2166</v>
       </c>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.25">
@@ -16097,10 +16220,10 @@
         <v>2141</v>
       </c>
       <c r="E259" s="10" t="s">
-        <v>2159</v>
+        <v>2157</v>
       </c>
       <c r="F259" s="5" t="s">
-        <v>2175</v>
+        <v>2176</v>
       </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.25">
@@ -16120,7 +16243,7 @@
         <v>599</v>
       </c>
       <c r="F260" s="5" t="s">
-        <v>2160</v>
+        <v>2158</v>
       </c>
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.25">
@@ -16140,7 +16263,7 @@
         <v>599</v>
       </c>
       <c r="F261" s="5" t="s">
-        <v>2176</v>
+        <v>2177</v>
       </c>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.25">
@@ -16157,10 +16280,10 @@
         <v>2122</v>
       </c>
       <c r="E262" s="10" t="s">
-        <v>2159</v>
+        <v>2157</v>
       </c>
       <c r="F262" s="5" t="s">
-        <v>2177</v>
+        <v>2167</v>
       </c>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.25">
@@ -16179,6 +16302,9 @@
       <c r="E263" s="10" t="s">
         <v>599</v>
       </c>
+      <c r="F263" s="5" t="s">
+        <v>2178</v>
+      </c>
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264">
@@ -16196,13 +16322,16 @@
       <c r="E264" s="10" t="s">
         <v>602</v>
       </c>
+      <c r="F264" s="5" t="s">
+        <v>2179</v>
+      </c>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>264</v>
       </c>
       <c r="B265" t="s">
-        <v>2161</v>
+        <v>2159</v>
       </c>
       <c r="C265" t="s">
         <v>2148</v>
@@ -16212,6 +16341,9 @@
       </c>
       <c r="E265" s="10" t="s">
         <v>599</v>
+      </c>
+      <c r="F265" s="5" t="s">
+        <v>2180</v>
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.25">
@@ -16230,6 +16362,9 @@
       <c r="E266" s="10" t="s">
         <v>602</v>
       </c>
+      <c r="F266" s="5" t="s">
+        <v>2181</v>
+      </c>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267">
@@ -16247,6 +16382,9 @@
       <c r="E267" s="10" t="s">
         <v>602</v>
       </c>
+      <c r="F267" s="5" t="s">
+        <v>2182</v>
+      </c>
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268">
@@ -16264,6 +16402,9 @@
       <c r="E268" s="10" t="s">
         <v>600</v>
       </c>
+      <c r="F268" s="5" t="s">
+        <v>2183</v>
+      </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269">
@@ -16279,7 +16420,10 @@
         <v>2116</v>
       </c>
       <c r="E269" s="10" t="s">
-        <v>2162</v>
+        <v>2160</v>
+      </c>
+      <c r="F269" s="5" t="s">
+        <v>2184</v>
       </c>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.25">
@@ -16298,6 +16442,9 @@
       <c r="E270" s="10" t="s">
         <v>600</v>
       </c>
+      <c r="F270" s="5" t="s">
+        <v>2185</v>
+      </c>
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271">
@@ -16315,6 +16462,9 @@
       <c r="E271" s="10" t="s">
         <v>602</v>
       </c>
+      <c r="F271" s="5" t="s">
+        <v>2186</v>
+      </c>
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272">
@@ -16330,10 +16480,13 @@
         <v>2</v>
       </c>
       <c r="E272" s="10" t="s">
-        <v>2159</v>
-      </c>
-    </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2157</v>
+      </c>
+      <c r="F272" s="5" t="s">
+        <v>2187</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>272</v>
       </c>
@@ -16347,10 +16500,13 @@
         <v>2</v>
       </c>
       <c r="E273" s="10" t="s">
-        <v>2159</v>
-      </c>
-    </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2157</v>
+      </c>
+      <c r="F273" s="5" t="s">
+        <v>2188</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>273</v>
       </c>
@@ -16364,10 +16520,13 @@
         <v>2</v>
       </c>
       <c r="E274" s="10" t="s">
-        <v>2159</v>
-      </c>
-    </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2157</v>
+      </c>
+      <c r="F274" s="5" t="s">
+        <v>2189</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>274</v>
       </c>
@@ -16381,10 +16540,13 @@
         <v>2116</v>
       </c>
       <c r="E275" s="10" t="s">
-        <v>2159</v>
-      </c>
-    </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2157</v>
+      </c>
+      <c r="F275" s="5" t="s">
+        <v>2190</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>275</v>
       </c>
@@ -16400,8 +16562,11 @@
       <c r="E276" s="10" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F276" s="5" t="s">
+        <v>2191</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>276</v>
       </c>
@@ -16417,8 +16582,11 @@
       <c r="E277" s="10" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F277" s="5" t="s">
+        <v>2192</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>277</v>
       </c>
@@ -16434,8 +16602,11 @@
       <c r="E278" s="10" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F278" s="5" t="s">
+        <v>2193</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>278</v>
       </c>
@@ -16449,10 +16620,13 @@
         <v>2116</v>
       </c>
       <c r="E279" s="10" t="s">
-        <v>2159</v>
-      </c>
-    </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2157</v>
+      </c>
+      <c r="F279" s="5" t="s">
+        <v>2194</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>279</v>
       </c>
@@ -16468,8 +16642,11 @@
       <c r="E280" s="10" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F280" s="5" t="s">
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>280</v>
       </c>
@@ -16483,10 +16660,13 @@
         <v>2</v>
       </c>
       <c r="E281" s="10" t="s">
-        <v>2159</v>
-      </c>
-    </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2157</v>
+      </c>
+      <c r="F281" s="5" t="s">
+        <v>2196</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>281</v>
       </c>
@@ -16502,8 +16682,11 @@
       <c r="E282" s="10" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F282" s="5" t="s">
+        <v>2197</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>282</v>
       </c>
@@ -16519,8 +16702,11 @@
       <c r="E283" s="10" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F283" s="5" t="s">
+        <v>2198</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>283</v>
       </c>
@@ -16534,10 +16720,13 @@
         <v>2</v>
       </c>
       <c r="E284" s="10" t="s">
-        <v>2159</v>
-      </c>
-    </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2157</v>
+      </c>
+      <c r="F284" s="5" t="s">
+        <v>2199</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>284</v>
       </c>
@@ -16553,13 +16742,16 @@
       <c r="E285" s="10" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F285" s="5" t="s">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>285</v>
       </c>
       <c r="B286" t="s">
-        <v>2163</v>
+        <v>2161</v>
       </c>
       <c r="C286" t="s">
         <v>2148</v>
@@ -16570,8 +16762,11 @@
       <c r="E286" s="10" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F286" s="5" t="s">
+        <v>2201</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>286</v>
       </c>
@@ -16587,8 +16782,11 @@
       <c r="E287" s="10" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F287" s="5" t="s">
+        <v>2202</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>287</v>
       </c>
@@ -16604,8 +16802,11 @@
       <c r="E288" s="10" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F288" s="5" t="s">
+        <v>2203</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>288</v>
       </c>
@@ -16619,10 +16820,13 @@
         <v>2116</v>
       </c>
       <c r="E289" s="10" t="s">
-        <v>2164</v>
-      </c>
-    </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2162</v>
+      </c>
+      <c r="F289" s="5" t="s">
+        <v>2204</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>289</v>
       </c>
@@ -16638,8 +16842,11 @@
       <c r="E290" s="10" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F290" s="5" t="s">
+        <v>2205</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>290</v>
       </c>
@@ -16655,8 +16862,11 @@
       <c r="E291" s="10" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F291" s="5" t="s">
+        <v>2206</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>291</v>
       </c>
@@ -16672,8 +16882,11 @@
       <c r="E292" s="10" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F292" s="5" t="s">
+        <v>2207</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>292</v>
       </c>
@@ -16689,8 +16902,11 @@
       <c r="E293" s="10" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F293" s="5" t="s">
+        <v>2208</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>293</v>
       </c>
@@ -16706,8 +16922,11 @@
       <c r="E294" s="10" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F294" s="5" t="s">
+        <v>2209</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>294</v>
       </c>
@@ -16723,8 +16942,11 @@
       <c r="E295" s="10" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F295" s="5" t="s">
+        <v>2210</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>295</v>
       </c>
@@ -16740,8 +16962,11 @@
       <c r="E296" s="10" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F296" s="5" t="s">
+        <v>2211</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>296</v>
       </c>
@@ -16757,13 +16982,16 @@
       <c r="E297" s="10" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F297" s="5" t="s">
+        <v>2212</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>297</v>
       </c>
       <c r="B298" t="s">
-        <v>2165</v>
+        <v>2163</v>
       </c>
       <c r="C298" t="s">
         <v>2148</v>
@@ -16772,10 +17000,13 @@
         <v>2141</v>
       </c>
       <c r="E298" s="10" t="s">
-        <v>2159</v>
-      </c>
-    </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2157</v>
+      </c>
+      <c r="F298" s="5" t="s">
+        <v>2213</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>298</v>
       </c>
@@ -16791,8 +17022,11 @@
       <c r="E299" s="10" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F299" s="5" t="s">
+        <v>2214</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>299</v>
       </c>
@@ -16808,8 +17042,11 @@
       <c r="E300" s="10" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F300" s="5" t="s">
+        <v>2215</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>300</v>
       </c>
@@ -16825,8 +17062,11 @@
       <c r="E301" s="10" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F301" s="5" t="s">
+        <v>2216</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>301</v>
       </c>
@@ -16840,10 +17080,13 @@
         <v>2139</v>
       </c>
       <c r="E302" s="10" t="s">
-        <v>2159</v>
-      </c>
-    </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2157</v>
+      </c>
+      <c r="F302" s="5" t="s">
+        <v>2217</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>302</v>
       </c>
@@ -16858,6 +17101,9 @@
       </c>
       <c r="E303" s="10" t="s">
         <v>602</v>
+      </c>
+      <c r="F303" s="5" t="s">
+        <v>2218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor fixes to raw card data.
</commit_message>
<xml_diff>
--- a/Data/Cards/DominionPickerData.xlsx
+++ b/Data/Cards/DominionPickerData.xlsx
@@ -7610,10 +7610,10 @@
   <dimension ref="A1:V303"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C240" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C172" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B246" sqref="B246:B303"/>
+      <selection pane="bottomRight" activeCell="D311" sqref="D311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Data file with 'Prizes' card. Include Prizes when picking Tournament. Made picker class static.
</commit_message>
<xml_diff>
--- a/Data/Cards/DominionPickerData.xlsx
+++ b/Data/Cards/DominionPickerData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\VSO\Veleek\Dominion Picker\Data\Cards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\VSO\Veleek\Dominion Picker\data\Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2985" uniqueCount="2219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2990" uniqueCount="2222">
   <si>
     <t>Cellar</t>
   </si>
@@ -6677,6 +6677,15 @@
   </si>
   <si>
     <t>+1 Buy\n+$4\nPut this on your Tavern mat.\n_____\nAt the end of your Buy phase, if you have at least $2 unspent, you may discard this from your Tavern mat.</t>
+  </si>
+  <si>
+    <t>Prizes</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Prizes are a set of five differently-named unique cards that are not part of the supply, but can be gained by playing Tournament.  They include Bag of Gold, Diadem, Followers, Princess, and Trusty Steed.</t>
   </si>
 </sst>
 </file>
@@ -7313,8 +7322,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:V303" totalsRowShown="0">
-  <autoFilter ref="A1:V303"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:V304" totalsRowShown="0">
+  <autoFilter ref="A1:V304"/>
   <tableColumns count="22">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Name"/>
@@ -7607,13 +7616,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:V303"/>
+  <dimension ref="A1:V304"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C172" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C293" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D311" sqref="D311"/>
+      <selection pane="bottomRight" activeCell="D304" sqref="D304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17104,6 +17113,26 @@
       </c>
       <c r="F303" s="5" t="s">
         <v>2218</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A304">
+        <v>303</v>
+      </c>
+      <c r="B304" t="s">
+        <v>2219</v>
+      </c>
+      <c r="C304" t="s">
+        <v>249</v>
+      </c>
+      <c r="D304" t="s">
+        <v>250</v>
+      </c>
+      <c r="E304" t="s">
+        <v>2220</v>
+      </c>
+      <c r="F304" s="5" t="s">
+        <v>2221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merging updated NL card names provided by Jeroen ter Heerdt <jeroen_ter_heerdt@hotmail.com>.
</commit_message>
<xml_diff>
--- a/Data/Cards/DominionPickerData.xlsx
+++ b/Data/Cards/DominionPickerData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\VSO\Veleek\Dominion Picker\data\Cards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\VSO\Veleek\Dominion Picker\Data\Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,12 +15,12 @@
     <sheet name="DominionPickerCards" sheetId="3" r:id="rId1"/>
     <sheet name="Groups" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2990" uniqueCount="2222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3113" uniqueCount="2325">
   <si>
     <t>Cellar</t>
   </si>
@@ -6686,12 +6686,321 @@
   </si>
   <si>
     <t>Prizes are a set of five differently-named unique cards that are not part of the supply, but can be gained by playing Tournament.  They include Bag of Gold, Diadem, Followers, Princess, and Trusty Steed.</t>
+  </si>
+  <si>
+    <t>Zak met goud</t>
+  </si>
+  <si>
+    <t>Tiara</t>
+  </si>
+  <si>
+    <t>Volgelingen</t>
+  </si>
+  <si>
+    <t>Prinses</t>
+  </si>
+  <si>
+    <t>Trouwe ros</t>
+  </si>
+  <si>
+    <t>Gehucht</t>
+  </si>
+  <si>
+    <t>Waarzegster</t>
+  </si>
+  <si>
+    <t>Boerendorp</t>
+  </si>
+  <si>
+    <t>Paardenhandelaars</t>
+  </si>
+  <si>
+    <t>Nieuwe versie</t>
+  </si>
+  <si>
+    <t>Toernooi</t>
+  </si>
+  <si>
+    <t>Jonge heks</t>
+  </si>
+  <si>
+    <t>Oogst</t>
+  </si>
+  <si>
+    <t>Hoorn des overvloeds</t>
+  </si>
+  <si>
+    <t>Jachtgezelschap</t>
+  </si>
+  <si>
+    <t>Nar</t>
+  </si>
+  <si>
+    <t>Kermisterrein</t>
+  </si>
+  <si>
+    <t>Splitsing</t>
+  </si>
+  <si>
+    <t>Hertogin</t>
+  </si>
+  <si>
+    <t>Klatergoud</t>
+  </si>
+  <si>
+    <t>Ontwikkelen</t>
+  </si>
+  <si>
+    <t>Gekonkel</t>
+  </si>
+  <si>
+    <t>Manusje-van-alles</t>
+  </si>
+  <si>
+    <t>Nobele bandiet</t>
+  </si>
+  <si>
+    <t>Nomadenkamp</t>
+  </si>
+  <si>
+    <t>Zijderoute</t>
+  </si>
+  <si>
+    <t>Specerijenkoopman</t>
+  </si>
+  <si>
+    <t>Handelaar</t>
+  </si>
+  <si>
+    <t>Bewaarplaats</t>
+  </si>
+  <si>
+    <t>Cartograaf</t>
+  </si>
+  <si>
+    <t>Sjacheraar</t>
+  </si>
+  <si>
+    <t>Hoofdweg</t>
+  </si>
+  <si>
+    <t>Gestolen goed</t>
+  </si>
+  <si>
+    <t>Herberg</t>
+  </si>
+  <si>
+    <t>Mandarijn</t>
+  </si>
+  <si>
+    <t>Markgraaf</t>
+  </si>
+  <si>
+    <t>Stallen</t>
+  </si>
+  <si>
+    <t>Grensdorp</t>
+  </si>
+  <si>
+    <t>Landbouwgrond</t>
+  </si>
+  <si>
+    <t>Verlaten mijn</t>
+  </si>
+  <si>
+    <t>Altaar</t>
+  </si>
+  <si>
+    <t>Wapenkamer</t>
+  </si>
+  <si>
+    <t>Groep mislukkelingen</t>
+  </si>
+  <si>
+    <t>Bandietenkamp</t>
+  </si>
+  <si>
+    <t>Bedelaar</t>
+  </si>
+  <si>
+    <t>Gewelven</t>
+  </si>
+  <si>
+    <t>Graaf</t>
+  </si>
+  <si>
+    <t>Vals geld</t>
+  </si>
+  <si>
+    <t>Dodenkar</t>
+  </si>
+  <si>
+    <t>Jager-verzamelaar</t>
+  </si>
+  <si>
+    <t>Vesting</t>
+  </si>
+  <si>
+    <t>Grafrover</t>
+  </si>
+  <si>
+    <t>Kluizenaar</t>
+  </si>
+  <si>
+    <t>Hutje</t>
+  </si>
+  <si>
+    <t>Jachtvelden</t>
+  </si>
+  <si>
+    <t>Metaalhandelaar</t>
+  </si>
+  <si>
+    <t>Opkoper</t>
+  </si>
+  <si>
+    <t>Ridders</t>
+  </si>
+  <si>
+    <t>Krankzinnige</t>
+  </si>
+  <si>
+    <t>Stroper</t>
+  </si>
+  <si>
+    <t>Marktplein</t>
+  </si>
+  <si>
+    <t>Huurling</t>
+  </si>
+  <si>
+    <t>Toverfeeks</t>
+  </si>
+  <si>
+    <t>Verwilderd landgoed</t>
+  </si>
+  <si>
+    <t>Plundering</t>
+  </si>
+  <si>
+    <t>Armenhuis</t>
+  </si>
+  <si>
+    <t>Optocht</t>
+  </si>
+  <si>
+    <t>Wederopbouw</t>
+  </si>
+  <si>
+    <t>Schurk</t>
+  </si>
+  <si>
+    <t>Ingestorte bibliotheek</t>
+  </si>
+  <si>
+    <t>Verwoeste markt</t>
+  </si>
+  <si>
+    <t>Vernield dorp</t>
+  </si>
+  <si>
+    <t>Ruïnes</t>
+  </si>
+  <si>
+    <t>Wijgeer</t>
+  </si>
+  <si>
+    <t>Scharrelaar</t>
+  </si>
+  <si>
+    <t>Buit</t>
+  </si>
+  <si>
+    <t>Schipknaap</t>
+  </si>
+  <si>
+    <t>Berghok</t>
+  </si>
+  <si>
+    <t>Overlevenden</t>
+  </si>
+  <si>
+    <t>Straatjongen</t>
+  </si>
+  <si>
+    <t>Landloper</t>
+  </si>
+  <si>
+    <t>Reizende minstreel</t>
+  </si>
+  <si>
+    <t>Onderdak</t>
+  </si>
+  <si>
+    <t>Adviseur</t>
+  </si>
+  <si>
+    <t>Bakker</t>
+  </si>
+  <si>
+    <t>Slager</t>
+  </si>
+  <si>
+    <t>Kandelaarmaker</t>
+  </si>
+  <si>
+    <t>Arts</t>
+  </si>
+  <si>
+    <t>Heraut</t>
+  </si>
+  <si>
+    <t>Gezel</t>
+  </si>
+  <si>
+    <t>Meesterwerk</t>
+  </si>
+  <si>
+    <t>Koopmansgilde</t>
+  </si>
+  <si>
+    <t>Helderziende</t>
+  </si>
+  <si>
+    <t>Steenhouwer</t>
+  </si>
+  <si>
+    <t>Belastinginner</t>
+  </si>
+  <si>
+    <t>Koper</t>
+  </si>
+  <si>
+    <t>Vloek</t>
+  </si>
+  <si>
+    <t>Landgoed</t>
+  </si>
+  <si>
+    <t>Zilver</t>
+  </si>
+  <si>
+    <t>Hertogdom</t>
+  </si>
+  <si>
+    <t>Goud</t>
+  </si>
+  <si>
+    <t>Provincie</t>
+  </si>
+  <si>
+    <t>Prijzen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -7428,6 +7737,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -7463,6 +7789,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -7619,10 +7962,10 @@
   <dimension ref="A1:V304"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C293" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K98" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D304" sqref="D304"/>
+      <selection pane="bottomRight" activeCell="Q104" sqref="Q104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12511,6 +12854,9 @@
       <c r="F118" s="5" t="s">
         <v>251</v>
       </c>
+      <c r="S118" s="1" t="s">
+        <v>2222</v>
+      </c>
     </row>
     <row r="119" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119">
@@ -12531,6 +12877,9 @@
       <c r="F119" s="5" t="s">
         <v>254</v>
       </c>
+      <c r="S119" s="1" t="s">
+        <v>2223</v>
+      </c>
     </row>
     <row r="120" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120">
@@ -12551,6 +12900,9 @@
       <c r="F120" s="5" t="s">
         <v>257</v>
       </c>
+      <c r="S120" s="1" t="s">
+        <v>2224</v>
+      </c>
     </row>
     <row r="121" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121">
@@ -12571,6 +12923,9 @@
       <c r="F121" s="5" t="s">
         <v>259</v>
       </c>
+      <c r="S121" s="1" t="s">
+        <v>2225</v>
+      </c>
     </row>
     <row r="122" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122">
@@ -12591,6 +12946,9 @@
       <c r="F122" s="5" t="s">
         <v>261</v>
       </c>
+      <c r="S122" s="1" t="s">
+        <v>2226</v>
+      </c>
     </row>
     <row r="123" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123">
@@ -12629,6 +12987,9 @@
       <c r="Q123" s="1" t="s">
         <v>718</v>
       </c>
+      <c r="S123" s="1" t="s">
+        <v>2227</v>
+      </c>
       <c r="U123" s="1" t="s">
         <v>719</v>
       </c>
@@ -12670,6 +13031,9 @@
       <c r="Q124" s="8" t="s">
         <v>2038</v>
       </c>
+      <c r="S124" s="1" t="s">
+        <v>2228</v>
+      </c>
       <c r="U124" s="8" t="s">
         <v>2039</v>
       </c>
@@ -12711,6 +13075,9 @@
       <c r="Q125" s="1" t="s">
         <v>757</v>
       </c>
+      <c r="S125" s="1" t="s">
+        <v>266</v>
+      </c>
       <c r="U125" s="1" t="s">
         <v>758</v>
       </c>
@@ -12752,6 +13119,9 @@
       <c r="Q126" s="1" t="s">
         <v>711</v>
       </c>
+      <c r="S126" s="1" t="s">
+        <v>2229</v>
+      </c>
       <c r="U126" s="1" t="s">
         <v>712</v>
       </c>
@@ -12793,6 +13163,9 @@
       <c r="Q127" s="1" t="s">
         <v>737</v>
       </c>
+      <c r="S127" s="1" t="s">
+        <v>2230</v>
+      </c>
       <c r="U127" s="1" t="s">
         <v>738</v>
       </c>
@@ -12834,6 +13207,9 @@
       <c r="Q128" s="1" t="s">
         <v>764</v>
       </c>
+      <c r="S128" s="1" t="s">
+        <v>2231</v>
+      </c>
       <c r="U128" s="1" t="s">
         <v>765</v>
       </c>
@@ -12875,6 +13251,9 @@
       <c r="Q129" s="1" t="s">
         <v>770</v>
       </c>
+      <c r="S129" s="1" t="s">
+        <v>2232</v>
+      </c>
       <c r="U129" s="1" t="s">
         <v>771</v>
       </c>
@@ -12916,6 +13295,9 @@
       <c r="Q130" s="1" t="s">
         <v>777</v>
       </c>
+      <c r="S130" s="1" t="s">
+        <v>2233</v>
+      </c>
       <c r="U130" s="1" t="s">
         <v>778</v>
       </c>
@@ -12957,6 +13339,9 @@
       <c r="Q131" s="1" t="s">
         <v>725</v>
       </c>
+      <c r="S131" s="1" t="s">
+        <v>2234</v>
+      </c>
       <c r="U131" s="1" t="s">
         <v>726</v>
       </c>
@@ -12998,6 +13383,9 @@
       <c r="Q132" s="1" t="s">
         <v>249</v>
       </c>
+      <c r="S132" s="1" t="s">
+        <v>2235</v>
+      </c>
       <c r="U132" s="1" t="s">
         <v>731</v>
       </c>
@@ -13039,6 +13427,9 @@
       <c r="Q133" s="1" t="s">
         <v>744</v>
       </c>
+      <c r="S133" s="1" t="s">
+        <v>2236</v>
+      </c>
       <c r="U133" s="1" t="s">
         <v>745</v>
       </c>
@@ -13080,6 +13471,9 @@
       <c r="Q134" s="1" t="s">
         <v>751</v>
       </c>
+      <c r="S134" s="1" t="s">
+        <v>2237</v>
+      </c>
       <c r="U134" s="1" t="s">
         <v>752</v>
       </c>
@@ -13121,6 +13515,9 @@
       <c r="Q135" s="1" t="s">
         <v>704</v>
       </c>
+      <c r="S135" s="1" t="s">
+        <v>2238</v>
+      </c>
       <c r="U135" s="1" t="s">
         <v>705</v>
       </c>
@@ -13150,6 +13547,9 @@
       <c r="O136" s="1" t="s">
         <v>787</v>
       </c>
+      <c r="S136" s="1" t="s">
+        <v>2239</v>
+      </c>
     </row>
     <row r="137" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137">
@@ -13176,6 +13576,9 @@
       <c r="O137" s="1" t="s">
         <v>791</v>
       </c>
+      <c r="S137" s="1" t="s">
+        <v>2240</v>
+      </c>
     </row>
     <row r="138" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138">
@@ -13202,6 +13605,9 @@
       <c r="O138" s="1" t="s">
         <v>797</v>
       </c>
+      <c r="S138" s="1" t="s">
+        <v>2241</v>
+      </c>
     </row>
     <row r="139" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139">
@@ -13228,6 +13634,9 @@
       <c r="O139" s="1" t="s">
         <v>789</v>
       </c>
+      <c r="S139" s="1" t="s">
+        <v>2242</v>
+      </c>
     </row>
     <row r="140" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140">
@@ -13254,6 +13663,9 @@
       <c r="O140" s="1" t="s">
         <v>298</v>
       </c>
+      <c r="S140" s="1" t="s">
+        <v>813</v>
+      </c>
     </row>
     <row r="141" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141">
@@ -13280,6 +13692,9 @@
       <c r="O141" s="1" t="s">
         <v>300</v>
       </c>
+      <c r="S141" s="1" t="s">
+        <v>814</v>
+      </c>
     </row>
     <row r="142" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142">
@@ -13306,6 +13721,9 @@
       <c r="O142" s="1" t="s">
         <v>816</v>
       </c>
+      <c r="S142" s="1" t="s">
+        <v>2243</v>
+      </c>
     </row>
     <row r="143" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143">
@@ -13332,6 +13750,9 @@
       <c r="O143" s="1" t="s">
         <v>304</v>
       </c>
+      <c r="S143" s="1" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="144" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144">
@@ -13358,8 +13779,11 @@
       <c r="O144" s="1" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="145" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S144" s="1" t="s">
+        <v>2244</v>
+      </c>
+    </row>
+    <row r="145" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -13384,8 +13808,11 @@
       <c r="O145" s="1" t="s">
         <v>810</v>
       </c>
-    </row>
-    <row r="146" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S145" s="1" t="s">
+        <v>2245</v>
+      </c>
+    </row>
+    <row r="146" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
@@ -13410,8 +13837,11 @@
       <c r="O146" s="1" t="s">
         <v>812</v>
       </c>
-    </row>
-    <row r="147" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S146" s="1" t="s">
+        <v>2246</v>
+      </c>
+    </row>
+    <row r="147" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
@@ -13436,8 +13866,11 @@
       <c r="O147" s="1" t="s">
         <v>818</v>
       </c>
-    </row>
-    <row r="148" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S147" s="1" t="s">
+        <v>2247</v>
+      </c>
+    </row>
+    <row r="148" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
@@ -13462,8 +13895,11 @@
       <c r="O148" s="1" t="s">
         <v>820</v>
       </c>
-    </row>
-    <row r="149" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S148" s="1" t="s">
+        <v>2248</v>
+      </c>
+    </row>
+    <row r="149" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
@@ -13488,8 +13924,11 @@
       <c r="O149" s="1" t="s">
         <v>824</v>
       </c>
-    </row>
-    <row r="150" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S149" s="1" t="s">
+        <v>2249</v>
+      </c>
+    </row>
+    <row r="150" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
@@ -13514,8 +13953,11 @@
       <c r="O150" s="1" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="151" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S150" s="1" t="s">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="151" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
@@ -13540,8 +13982,11 @@
       <c r="O151" s="1" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="152" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S151" s="1" t="s">
+        <v>2251</v>
+      </c>
+    </row>
+    <row r="152" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
@@ -13566,8 +14011,11 @@
       <c r="O152" s="1" t="s">
         <v>793</v>
       </c>
-    </row>
-    <row r="153" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S152" s="1" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="153" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
@@ -13592,8 +14040,11 @@
       <c r="O153" s="1" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="154" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S153" s="1" t="s">
+        <v>2252</v>
+      </c>
+    </row>
+    <row r="154" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
@@ -13618,8 +14069,11 @@
       <c r="O154" s="1" t="s">
         <v>801</v>
       </c>
-    </row>
-    <row r="155" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S154" s="1" t="s">
+        <v>2253</v>
+      </c>
+    </row>
+    <row r="155" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
@@ -13644,8 +14098,11 @@
       <c r="O155" s="1" t="s">
         <v>803</v>
       </c>
-    </row>
-    <row r="156" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S155" s="1" t="s">
+        <v>2254</v>
+      </c>
+    </row>
+    <row r="156" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
@@ -13670,8 +14127,11 @@
       <c r="O156" s="1" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="157" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S156" s="1" t="s">
+        <v>2255</v>
+      </c>
+    </row>
+    <row r="157" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
@@ -13696,8 +14156,11 @@
       <c r="O157" s="1" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="158" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S157" s="1" t="s">
+        <v>2256</v>
+      </c>
+    </row>
+    <row r="158" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -13722,8 +14185,11 @@
       <c r="O158" s="1" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="159" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S158" s="1" t="s">
+        <v>2257</v>
+      </c>
+    </row>
+    <row r="159" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
@@ -13748,8 +14214,11 @@
       <c r="O159" s="1" t="s">
         <v>822</v>
       </c>
-    </row>
-    <row r="160" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S159" s="1" t="s">
+        <v>2258</v>
+      </c>
+    </row>
+    <row r="160" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
@@ -13773,6 +14242,9 @@
       </c>
       <c r="O160" s="1" t="s">
         <v>782</v>
+      </c>
+      <c r="S160" s="1" t="s">
+        <v>2259</v>
       </c>
     </row>
     <row r="161" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -13800,6 +14272,9 @@
       <c r="O161" s="1" t="s">
         <v>795</v>
       </c>
+      <c r="S161" s="1" t="s">
+        <v>2260</v>
+      </c>
     </row>
     <row r="162" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162">
@@ -13998,6 +14473,9 @@
       <c r="J167" s="5" t="s">
         <v>562</v>
       </c>
+      <c r="S167" s="1" t="s">
+        <v>2261</v>
+      </c>
     </row>
     <row r="168" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168">
@@ -14024,6 +14502,9 @@
       <c r="J168" s="5" t="s">
         <v>2046</v>
       </c>
+      <c r="S168" s="1" t="s">
+        <v>2262</v>
+      </c>
     </row>
     <row r="169" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169">
@@ -14050,6 +14531,9 @@
       <c r="J169" s="5" t="s">
         <v>2047</v>
       </c>
+      <c r="S169" s="1" t="s">
+        <v>2263</v>
+      </c>
     </row>
     <row r="170" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170">
@@ -14076,6 +14560,9 @@
       <c r="J170" s="5" t="s">
         <v>2048</v>
       </c>
+      <c r="S170" s="1" t="s">
+        <v>2264</v>
+      </c>
     </row>
     <row r="171" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171">
@@ -14102,6 +14589,9 @@
       <c r="J171" s="5" t="s">
         <v>2050</v>
       </c>
+      <c r="S171" s="1" t="s">
+        <v>2265</v>
+      </c>
     </row>
     <row r="172" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172">
@@ -14128,6 +14618,9 @@
       <c r="J172" s="5" t="s">
         <v>2051</v>
       </c>
+      <c r="S172" s="1" t="s">
+        <v>2266</v>
+      </c>
     </row>
     <row r="173" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173">
@@ -14154,6 +14647,9 @@
       <c r="J173" s="5" t="s">
         <v>2052</v>
       </c>
+      <c r="S173" s="1" t="s">
+        <v>2267</v>
+      </c>
     </row>
     <row r="174" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174">
@@ -14180,6 +14676,9 @@
       <c r="J174" s="5" t="s">
         <v>2053</v>
       </c>
+      <c r="S174" s="1" t="s">
+        <v>2268</v>
+      </c>
     </row>
     <row r="175" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175">
@@ -14206,6 +14705,9 @@
       <c r="J175" s="5" t="s">
         <v>2054</v>
       </c>
+      <c r="S175" s="1" t="s">
+        <v>2269</v>
+      </c>
     </row>
     <row r="176" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176">
@@ -14232,8 +14734,11 @@
       <c r="J176" s="5" t="s">
         <v>2055</v>
       </c>
-    </row>
-    <row r="177" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S176" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="177" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
       </c>
@@ -14258,8 +14763,11 @@
       <c r="J177" s="5" t="s">
         <v>2056</v>
       </c>
-    </row>
-    <row r="178" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S177" s="1" t="s">
+        <v>2270</v>
+      </c>
+    </row>
+    <row r="178" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>177</v>
       </c>
@@ -14284,8 +14792,11 @@
       <c r="J178" s="5" t="s">
         <v>2057</v>
       </c>
-    </row>
-    <row r="179" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S178" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="179" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>178</v>
       </c>
@@ -14310,8 +14821,11 @@
       <c r="J179" s="5" t="s">
         <v>2058</v>
       </c>
-    </row>
-    <row r="180" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S179" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="180" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>179</v>
       </c>
@@ -14336,8 +14850,11 @@
       <c r="J180" s="5" t="s">
         <v>2059</v>
       </c>
-    </row>
-    <row r="181" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S180" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="181" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>180</v>
       </c>
@@ -14362,8 +14879,11 @@
       <c r="J181" s="5" t="s">
         <v>2060</v>
       </c>
-    </row>
-    <row r="182" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S181" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="182" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>181</v>
       </c>
@@ -14388,8 +14908,11 @@
       <c r="J182" s="5" t="s">
         <v>2061</v>
       </c>
-    </row>
-    <row r="183" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S182" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="183" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>182</v>
       </c>
@@ -14414,8 +14937,11 @@
       <c r="J183" s="5" t="s">
         <v>2062</v>
       </c>
-    </row>
-    <row r="184" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S183" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="184" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>183</v>
       </c>
@@ -14440,8 +14966,11 @@
       <c r="J184" s="5" t="s">
         <v>2063</v>
       </c>
-    </row>
-    <row r="185" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S184" s="1" t="s">
+        <v>2271</v>
+      </c>
+    </row>
+    <row r="185" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>184</v>
       </c>
@@ -14466,8 +14995,11 @@
       <c r="J185" s="5" t="s">
         <v>2064</v>
       </c>
-    </row>
-    <row r="186" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S185" s="1" t="s">
+        <v>2272</v>
+      </c>
+    </row>
+    <row r="186" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>185</v>
       </c>
@@ -14492,8 +15024,11 @@
       <c r="J186" s="5" t="s">
         <v>2065</v>
       </c>
-    </row>
-    <row r="187" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S186" s="1" t="s">
+        <v>2273</v>
+      </c>
+    </row>
+    <row r="187" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>186</v>
       </c>
@@ -14518,8 +15053,11 @@
       <c r="J187" s="5" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="188" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S187" s="1" t="s">
+        <v>2274</v>
+      </c>
+    </row>
+    <row r="188" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>187</v>
       </c>
@@ -14544,8 +15082,11 @@
       <c r="J188" s="5" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="189" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S188" s="1" t="s">
+        <v>2275</v>
+      </c>
+    </row>
+    <row r="189" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>188</v>
       </c>
@@ -14570,8 +15111,11 @@
       <c r="J189" s="5" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="190" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S189" s="1" t="s">
+        <v>2276</v>
+      </c>
+    </row>
+    <row r="190" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>189</v>
       </c>
@@ -14596,8 +15140,11 @@
       <c r="J190" s="5" t="s">
         <v>2033</v>
       </c>
-    </row>
-    <row r="191" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S190" s="1" t="s">
+        <v>2277</v>
+      </c>
+    </row>
+    <row r="191" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>190</v>
       </c>
@@ -14622,8 +15169,11 @@
       <c r="J191" s="5" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="192" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S191" s="1" t="s">
+        <v>2278</v>
+      </c>
+    </row>
+    <row r="192" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>191</v>
       </c>
@@ -14645,8 +15195,11 @@
       <c r="I192" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="193" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S192" s="1" t="s">
+        <v>2279</v>
+      </c>
+    </row>
+    <row r="193" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>192</v>
       </c>
@@ -14671,8 +15224,11 @@
       <c r="J193" s="5" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="194" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S193" s="1" t="s">
+        <v>2280</v>
+      </c>
+    </row>
+    <row r="194" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>193</v>
       </c>
@@ -14697,8 +15253,11 @@
       <c r="J194" s="5" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="195" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S194" s="1" t="s">
+        <v>2281</v>
+      </c>
+    </row>
+    <row r="195" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>194</v>
       </c>
@@ -14723,8 +15282,11 @@
       <c r="J195" s="5" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="196" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S195" s="1" t="s">
+        <v>2282</v>
+      </c>
+    </row>
+    <row r="196" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>195</v>
       </c>
@@ -14749,8 +15311,11 @@
       <c r="J196" s="5" t="s">
         <v>2049</v>
       </c>
-    </row>
-    <row r="197" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S196" s="1" t="s">
+        <v>2283</v>
+      </c>
+    </row>
+    <row r="197" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>196</v>
       </c>
@@ -14775,8 +15340,11 @@
       <c r="J197" s="5" t="s">
         <v>2066</v>
       </c>
-    </row>
-    <row r="198" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S197" s="1" t="s">
+        <v>2284</v>
+      </c>
+    </row>
+    <row r="198" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>197</v>
       </c>
@@ -14801,8 +15369,11 @@
       <c r="J198" s="5" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="199" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S198" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="199" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>198</v>
       </c>
@@ -14827,8 +15398,11 @@
       <c r="J199" s="5" t="s">
         <v>2067</v>
       </c>
-    </row>
-    <row r="200" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S199" s="1" t="s">
+        <v>2285</v>
+      </c>
+    </row>
+    <row r="200" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>199</v>
       </c>
@@ -14853,8 +15427,11 @@
       <c r="J200" s="5" t="s">
         <v>2068</v>
       </c>
-    </row>
-    <row r="201" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S200" s="1" t="s">
+        <v>2286</v>
+      </c>
+    </row>
+    <row r="201" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>200</v>
       </c>
@@ -14879,8 +15456,11 @@
       <c r="J201" s="5" t="s">
         <v>2069</v>
       </c>
-    </row>
-    <row r="202" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S201" s="1" t="s">
+        <v>2287</v>
+      </c>
+    </row>
+    <row r="202" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>201</v>
       </c>
@@ -14905,8 +15485,11 @@
       <c r="J202" s="5" t="s">
         <v>2070</v>
       </c>
-    </row>
-    <row r="203" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S202" s="1" t="s">
+        <v>2288</v>
+      </c>
+    </row>
+    <row r="203" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>202</v>
       </c>
@@ -14931,8 +15514,11 @@
       <c r="J203" s="5" t="s">
         <v>2071</v>
       </c>
-    </row>
-    <row r="204" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S203" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="204" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>203</v>
       </c>
@@ -14957,8 +15543,11 @@
       <c r="J204" s="5" t="s">
         <v>2072</v>
       </c>
-    </row>
-    <row r="205" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S204" s="1" t="s">
+        <v>2289</v>
+      </c>
+    </row>
+    <row r="205" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>204</v>
       </c>
@@ -14983,8 +15572,11 @@
       <c r="J205" s="5" t="s">
         <v>2073</v>
       </c>
-    </row>
-    <row r="206" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S205" s="1" t="s">
+        <v>2290</v>
+      </c>
+    </row>
+    <row r="206" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>205</v>
       </c>
@@ -15009,8 +15601,11 @@
       <c r="J206" s="5" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="207" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S206" s="1" t="s">
+        <v>2291</v>
+      </c>
+    </row>
+    <row r="207" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>206</v>
       </c>
@@ -15035,8 +15630,11 @@
       <c r="J207" s="5" t="s">
         <v>572</v>
       </c>
-    </row>
-    <row r="208" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S207" s="1" t="s">
+        <v>2292</v>
+      </c>
+    </row>
+    <row r="208" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>207</v>
       </c>
@@ -15061,8 +15659,11 @@
       <c r="J208" s="5" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="209" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S208" s="1" t="s">
+        <v>2293</v>
+      </c>
+    </row>
+    <row r="209" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>208</v>
       </c>
@@ -15084,8 +15685,11 @@
       <c r="I209" s="1" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="210" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S209" s="1" t="s">
+        <v>2294</v>
+      </c>
+    </row>
+    <row r="210" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>209</v>
       </c>
@@ -15110,8 +15714,11 @@
       <c r="J210" s="5" t="s">
         <v>2074</v>
       </c>
-    </row>
-    <row r="211" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S210" s="1" t="s">
+        <v>2295</v>
+      </c>
+    </row>
+    <row r="211" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>210</v>
       </c>
@@ -15136,8 +15743,11 @@
       <c r="J211" s="5" t="s">
         <v>2075</v>
       </c>
-    </row>
-    <row r="212" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S211" s="1" t="s">
+        <v>2296</v>
+      </c>
+    </row>
+    <row r="212" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>211</v>
       </c>
@@ -15162,8 +15772,11 @@
       <c r="J212" s="5" t="s">
         <v>2076</v>
       </c>
-    </row>
-    <row r="213" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S212" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="213" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>212</v>
       </c>
@@ -15188,8 +15801,11 @@
       <c r="J213" s="5" t="s">
         <v>2077</v>
       </c>
-    </row>
-    <row r="214" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S213" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="214" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>213</v>
       </c>
@@ -15214,8 +15830,11 @@
       <c r="J214" s="5" t="s">
         <v>2078</v>
       </c>
-    </row>
-    <row r="215" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S214" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="215" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>214</v>
       </c>
@@ -15240,8 +15859,11 @@
       <c r="J215" s="5" t="s">
         <v>2079</v>
       </c>
-    </row>
-    <row r="216" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S215" s="1" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="216" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>215</v>
       </c>
@@ -15266,8 +15888,11 @@
       <c r="J216" s="5" t="s">
         <v>2080</v>
       </c>
-    </row>
-    <row r="217" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S216" s="1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="217" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>216</v>
       </c>
@@ -15292,8 +15917,11 @@
       <c r="J217" s="6" t="s">
         <v>2081</v>
       </c>
-    </row>
-    <row r="218" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S217" s="1" t="s">
+        <v>2297</v>
+      </c>
+    </row>
+    <row r="218" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>217</v>
       </c>
@@ -15318,8 +15946,11 @@
       <c r="J218" s="5" t="s">
         <v>2082</v>
       </c>
-    </row>
-    <row r="219" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S218" s="1" t="s">
+        <v>2298</v>
+      </c>
+    </row>
+    <row r="219" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>218</v>
       </c>
@@ -15344,8 +15975,11 @@
       <c r="J219" s="5" t="s">
         <v>2083</v>
       </c>
-    </row>
-    <row r="220" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S219" s="1" t="s">
+        <v>2299</v>
+      </c>
+    </row>
+    <row r="220" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>219</v>
       </c>
@@ -15370,8 +16004,11 @@
       <c r="J220" s="5" t="s">
         <v>2084</v>
       </c>
-    </row>
-    <row r="221" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S220" s="1" t="s">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="221" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>220</v>
       </c>
@@ -15396,8 +16033,11 @@
       <c r="J221" s="5" t="s">
         <v>2085</v>
       </c>
-    </row>
-    <row r="222" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S221" s="1" t="s">
+        <v>2301</v>
+      </c>
+    </row>
+    <row r="222" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>221</v>
       </c>
@@ -15422,8 +16062,11 @@
       <c r="J222" s="5" t="s">
         <v>2086</v>
       </c>
-    </row>
-    <row r="223" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S222" s="1" t="s">
+        <v>2302</v>
+      </c>
+    </row>
+    <row r="223" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>222</v>
       </c>
@@ -15448,8 +16091,11 @@
       <c r="J223" s="5" t="s">
         <v>2087</v>
       </c>
-    </row>
-    <row r="224" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S223" s="1" t="s">
+        <v>2303</v>
+      </c>
+    </row>
+    <row r="224" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>223</v>
       </c>
@@ -15471,8 +16117,11 @@
       <c r="I224" s="1" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="225" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S224" s="1" t="s">
+        <v>2304</v>
+      </c>
+    </row>
+    <row r="225" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>224</v>
       </c>
@@ -15494,8 +16143,11 @@
       <c r="I225" s="1" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="226" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S225" s="1" t="s">
+        <v>2305</v>
+      </c>
+    </row>
+    <row r="226" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>225</v>
       </c>
@@ -15517,8 +16169,11 @@
       <c r="I226" s="1" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="227" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S226" s="1" t="s">
+        <v>2306</v>
+      </c>
+    </row>
+    <row r="227" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>226</v>
       </c>
@@ -15540,8 +16195,11 @@
       <c r="I227" s="1" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="228" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S227" s="1" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="228" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>227</v>
       </c>
@@ -15563,8 +16221,11 @@
       <c r="I228" s="1" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="229" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S228" s="1" t="s">
+        <v>2308</v>
+      </c>
+    </row>
+    <row r="229" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>228</v>
       </c>
@@ -15586,8 +16247,11 @@
       <c r="I229" s="1" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="230" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S229" s="1" t="s">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="230" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>229</v>
       </c>
@@ -15609,8 +16273,11 @@
       <c r="I230" s="1" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="231" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S230" s="1" t="s">
+        <v>2310</v>
+      </c>
+    </row>
+    <row r="231" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>230</v>
       </c>
@@ -15632,8 +16299,11 @@
       <c r="I231" s="1" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="232" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S231" s="1" t="s">
+        <v>2311</v>
+      </c>
+    </row>
+    <row r="232" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>231</v>
       </c>
@@ -15655,8 +16325,11 @@
       <c r="I232" s="1" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="233" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S232" s="1" t="s">
+        <v>2312</v>
+      </c>
+    </row>
+    <row r="233" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>232</v>
       </c>
@@ -15678,8 +16351,11 @@
       <c r="I233" s="1" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="234" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S233" s="1" t="s">
+        <v>2313</v>
+      </c>
+    </row>
+    <row r="234" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>233</v>
       </c>
@@ -15701,8 +16377,11 @@
       <c r="I234" s="1" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="235" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S234" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="235" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>234</v>
       </c>
@@ -15724,8 +16403,11 @@
       <c r="I235" s="1" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="236" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S235" s="1" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="236" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>235</v>
       </c>
@@ -15747,8 +16429,11 @@
       <c r="I236" s="1" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="237" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S236" s="1" t="s">
+        <v>2315</v>
+      </c>
+    </row>
+    <row r="237" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>236</v>
       </c>
@@ -15770,8 +16455,11 @@
       <c r="I237" s="1" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="238" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S237" s="1" t="s">
+        <v>2316</v>
+      </c>
+    </row>
+    <row r="238" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>237</v>
       </c>
@@ -15794,7 +16482,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="239" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>238</v>
       </c>
@@ -15816,8 +16504,11 @@
       <c r="O239" s="1" t="s">
         <v>2042</v>
       </c>
-    </row>
-    <row r="240" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S239" s="1" t="s">
+        <v>2317</v>
+      </c>
+    </row>
+    <row r="240" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>239</v>
       </c>
@@ -15839,8 +16530,11 @@
       <c r="O240" s="1" t="s">
         <v>2044</v>
       </c>
-    </row>
-    <row r="241" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S240" s="1" t="s">
+        <v>2318</v>
+      </c>
+    </row>
+    <row r="241" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>240</v>
       </c>
@@ -15862,8 +16556,11 @@
       <c r="O241" s="1" t="s">
         <v>2043</v>
       </c>
-    </row>
-    <row r="242" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S241" s="1" t="s">
+        <v>2319</v>
+      </c>
+    </row>
+    <row r="242" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>241</v>
       </c>
@@ -15885,8 +16582,11 @@
       <c r="O242" s="1" t="s">
         <v>2041</v>
       </c>
-    </row>
-    <row r="243" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S242" s="1" t="s">
+        <v>2320</v>
+      </c>
+    </row>
+    <row r="243" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>242</v>
       </c>
@@ -15908,8 +16608,11 @@
       <c r="O243" s="1" t="s">
         <v>2045</v>
       </c>
-    </row>
-    <row r="244" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S243" s="1" t="s">
+        <v>2321</v>
+      </c>
+    </row>
+    <row r="244" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>243</v>
       </c>
@@ -15931,8 +16634,11 @@
       <c r="O244" s="1" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="245" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S244" s="1" t="s">
+        <v>2322</v>
+      </c>
+    </row>
+    <row r="245" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>244</v>
       </c>
@@ -15951,8 +16657,11 @@
       <c r="F245" s="5" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="246" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S245" s="1" t="s">
+        <v>2323</v>
+      </c>
+    </row>
+    <row r="246" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>245</v>
       </c>
@@ -15975,7 +16684,7 @@
         <v>2155</v>
       </c>
     </row>
-    <row r="247" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>246</v>
       </c>
@@ -15995,7 +16704,7 @@
         <v>2168</v>
       </c>
     </row>
-    <row r="248" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>247</v>
       </c>
@@ -16015,7 +16724,7 @@
         <v>2169</v>
       </c>
     </row>
-    <row r="249" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>248</v>
       </c>
@@ -16035,7 +16744,7 @@
         <v>2170</v>
       </c>
     </row>
-    <row r="250" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>249</v>
       </c>
@@ -16055,7 +16764,7 @@
         <v>2156</v>
       </c>
     </row>
-    <row r="251" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>250</v>
       </c>
@@ -16075,7 +16784,7 @@
         <v>2171</v>
       </c>
     </row>
-    <row r="252" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>251</v>
       </c>
@@ -16095,7 +16804,7 @@
         <v>2172</v>
       </c>
     </row>
-    <row r="253" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>252</v>
       </c>
@@ -16115,7 +16824,7 @@
         <v>2173</v>
       </c>
     </row>
-    <row r="254" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>253</v>
       </c>
@@ -16135,7 +16844,7 @@
         <v>2164</v>
       </c>
     </row>
-    <row r="255" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>254</v>
       </c>
@@ -16155,7 +16864,7 @@
         <v>2174</v>
       </c>
     </row>
-    <row r="256" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>255</v>
       </c>
@@ -16815,7 +17524,7 @@
         <v>2203</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>288</v>
       </c>
@@ -16835,7 +17544,7 @@
         <v>2204</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>289</v>
       </c>
@@ -16855,7 +17564,7 @@
         <v>2205</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>290</v>
       </c>
@@ -16875,7 +17584,7 @@
         <v>2206</v>
       </c>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>291</v>
       </c>
@@ -16895,7 +17604,7 @@
         <v>2207</v>
       </c>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>292</v>
       </c>
@@ -16915,7 +17624,7 @@
         <v>2208</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>293</v>
       </c>
@@ -16935,7 +17644,7 @@
         <v>2209</v>
       </c>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>294</v>
       </c>
@@ -16955,7 +17664,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>295</v>
       </c>
@@ -16975,7 +17684,7 @@
         <v>2211</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>296</v>
       </c>
@@ -16995,7 +17704,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>297</v>
       </c>
@@ -17015,7 +17724,7 @@
         <v>2213</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>298</v>
       </c>
@@ -17035,7 +17744,7 @@
         <v>2214</v>
       </c>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>299</v>
       </c>
@@ -17055,7 +17764,7 @@
         <v>2215</v>
       </c>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>300</v>
       </c>
@@ -17075,7 +17784,7 @@
         <v>2216</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>301</v>
       </c>
@@ -17095,7 +17804,7 @@
         <v>2217</v>
       </c>
     </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>302</v>
       </c>
@@ -17115,7 +17824,7 @@
         <v>2218</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>303</v>
       </c>
@@ -17133,6 +17842,9 @@
       </c>
       <c r="F304" s="5" t="s">
         <v>2221</v>
+      </c>
+      <c r="S304" s="1" t="s">
+        <v>2324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major functionality walkthrough fixes
General walkthrough to fix existing features.
Fixed localization stuff to use a different RESW generator that allows
changing culture manually.
Fixed up bugs in CardInfo page.
Added 2nd Edition sets.
Fixed up About pages.
</commit_message>
<xml_diff>
--- a/Data/Cards/DominionPickerData.xlsx
+++ b/Data/Cards/DominionPickerData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17668"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\VSO\Veleek\Dominion Picker\Data\Cards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\src\vso\Veleek\Dominion Picker\Data\Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,14 +13,15 @@
   </bookViews>
   <sheets>
     <sheet name="DominionPickerCards" sheetId="3" r:id="rId1"/>
-    <sheet name="Groups" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
+    <sheet name="Groups" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3845" uniqueCount="2536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4008" uniqueCount="2577">
   <si>
     <t>Cellar</t>
   </si>
@@ -7628,6 +7629,129 @@
   </si>
   <si>
     <t>Move your -$2 cost token to an Action Supply pile (cards from that pile cost $2 less on your turns, but not less than $0).</t>
+  </si>
+  <si>
+    <t>Merchant</t>
+  </si>
+  <si>
+    <t>Harbinger</t>
+  </si>
+  <si>
+    <t>Vassal</t>
+  </si>
+  <si>
+    <t>Discard the top card of your deck. If it is an Action card, you may play it.</t>
+  </si>
+  <si>
+    <t>Artisan</t>
+  </si>
+  <si>
+    <t>Sentry</t>
+  </si>
+  <si>
+    <t>2?</t>
+  </si>
+  <si>
+    <t>Poacher</t>
+  </si>
+  <si>
+    <t>+1,-X</t>
+  </si>
+  <si>
+    <t>Bandit</t>
+  </si>
+  <si>
+    <t>Gain a Gold. Each other player reveals the top 2 cards of their deck, trashes a revealed treasure other than Copper, and discards the rest.</t>
+  </si>
+  <si>
+    <t>Base2E</t>
+  </si>
+  <si>
+    <t>Lurker</t>
+  </si>
+  <si>
+    <t>1?</t>
+  </si>
+  <si>
+    <t>Mill</t>
+  </si>
+  <si>
+    <t>+1,-2?</t>
+  </si>
+  <si>
+    <t>Diplomat</t>
+  </si>
+  <si>
+    <t>+2 Cards. If you have 5 or fewer cards in hand (after drawing), +2 Actions. — When another player plays an Attack card, you may first reveal this from a hand of 5 or more cards, to draw 2 cards then discard 3.</t>
+  </si>
+  <si>
+    <t>+2?</t>
+  </si>
+  <si>
+    <t>Patrol</t>
+  </si>
+  <si>
+    <t>+3 Cards. Reveal the top 4 cards of your deck. Put the Victory cards and Curses into your hand. Put the rest back in any order.</t>
+  </si>
+  <si>
+    <t>Replace</t>
+  </si>
+  <si>
+    <t>Secret Passage</t>
+  </si>
+  <si>
+    <t>+2,-1</t>
+  </si>
+  <si>
+    <t>Courtier</t>
+  </si>
+  <si>
+    <t>+1?</t>
+  </si>
+  <si>
+    <t>Intrigue2E</t>
+  </si>
+  <si>
+    <t>+1 Card\n+1 Action\nLook through your discard pile. You may put a card from it onto your deck.</t>
+  </si>
+  <si>
+    <t>+1 Card\n+1 Action\nLook at the top 2 cards of your deck. Trash and/or discard any number of them. Put the rest back in any order.</t>
+  </si>
+  <si>
+    <t>+1 Action\nChoose one: Trash an Action card from the Supply, or gain an Action card from the trash.</t>
+  </si>
+  <si>
+    <t>+2 Cards\n+1 Action\nTake a card from your hand and put it anywhere in your deck.</t>
+  </si>
+  <si>
+    <t>+1 Card\n+1 Action\nThe first time you play a Silver this turn, +$1.</t>
+  </si>
+  <si>
+    <t>Gain a card to your hand costing up to $5. Put a card from your hand onto your deck.</t>
+  </si>
+  <si>
+    <t>+1 Card\n+1 Action\n+$1. Discard a card per empty supply pile.</t>
+  </si>
+  <si>
+    <t>+1 Card\n+1 Action\nYou may discard 2 cards, for +$2. Worth 1VP</t>
+  </si>
+  <si>
+    <t>Trash a card from your hand. Gain a card costing up to $2 more than it. If the gained card is an Action or Treasure, put it onto your deck; if it's a Victory card, each other player gains a Curse.</t>
+  </si>
+  <si>
+    <t>Reveal a card from your hand. For each type it has (Action, Attack, etc.), choose one: +1 Action; or +1 Buy; or +$3; or gain a Gold. The choices must be different.</t>
+  </si>
+  <si>
+    <t>Sauna</t>
+  </si>
+  <si>
+    <t>+1 Card\n+1 Action\nYou may play an Avanto from your hand. — While this is in play, when you play a Silver, you may trash a card from your hand.</t>
+  </si>
+  <si>
+    <t>+3 Cards. You may play an Sauna from your hand.</t>
+  </si>
+  <si>
+    <t>Avanto</t>
   </si>
 </sst>
 </file>
@@ -8270,8 +8394,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:W376" totalsRowShown="0">
-  <autoFilter ref="A1:W376"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:W392" totalsRowShown="0">
+  <autoFilter ref="A1:W392"/>
   <sortState ref="A2:W376">
     <sortCondition ref="A1:A376"/>
   </sortState>
@@ -8602,38 +8726,38 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:W376"/>
+  <dimension ref="A1:W392"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A354" workbookViewId="0">
       <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G118" sqref="G118"/>
+      <selection pane="topRight" activeCell="G373" sqref="G373"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.25" customWidth="1"/>
-    <col min="7" max="7" width="211.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="18.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" customWidth="1"/>
+    <col min="7" max="7" width="211.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -19633,7 +19757,7 @@
       <c r="F306" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G306" t="s">
+      <c r="G306" s="10" t="s">
         <v>2521</v>
       </c>
     </row>
@@ -19656,7 +19780,7 @@
       <c r="F307" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G307" t="s">
+      <c r="G307" s="10" t="s">
         <v>2450</v>
       </c>
     </row>
@@ -19677,7 +19801,7 @@
       <c r="F308" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G308" t="s">
+      <c r="G308" s="10" t="s">
         <v>2472</v>
       </c>
     </row>
@@ -19700,7 +19824,7 @@
       <c r="F309" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G309" t="s">
+      <c r="G309" s="10" t="s">
         <v>2452</v>
       </c>
     </row>
@@ -19721,7 +19845,7 @@
       <c r="F310" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G310" t="s">
+      <c r="G310" s="10" t="s">
         <v>2473</v>
       </c>
     </row>
@@ -19742,7 +19866,7 @@
       <c r="F311" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G311" t="s">
+      <c r="G311" s="10" t="s">
         <v>2474</v>
       </c>
     </row>
@@ -19765,7 +19889,7 @@
       <c r="F312" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G312" t="s">
+      <c r="G312" s="10" t="s">
         <v>2522</v>
       </c>
     </row>
@@ -19786,7 +19910,7 @@
       <c r="F313" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G313" t="s">
+      <c r="G313" s="10" t="s">
         <v>2523</v>
       </c>
     </row>
@@ -19807,7 +19931,7 @@
       <c r="F314" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G314" t="s">
+      <c r="G314" s="10" t="s">
         <v>2475</v>
       </c>
     </row>
@@ -19828,7 +19952,7 @@
       <c r="F315" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G315" t="s">
+      <c r="G315" s="10" t="s">
         <v>2476</v>
       </c>
     </row>
@@ -19851,7 +19975,7 @@
       <c r="F316" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G316" t="s">
+      <c r="G316" s="10" t="s">
         <v>2453</v>
       </c>
     </row>
@@ -19874,7 +19998,7 @@
       <c r="F317" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G317" t="s">
+      <c r="G317" s="10" t="s">
         <v>2524</v>
       </c>
     </row>
@@ -19897,7 +20021,7 @@
       <c r="F318" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G318" t="s">
+      <c r="G318" s="10" t="s">
         <v>2455</v>
       </c>
     </row>
@@ -19920,7 +20044,7 @@
       <c r="F319" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G319" t="s">
+      <c r="G319" s="10" t="s">
         <v>2525</v>
       </c>
     </row>
@@ -19943,7 +20067,7 @@
       <c r="F320" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G320" t="s">
+      <c r="G320" s="10" t="s">
         <v>2477</v>
       </c>
     </row>
@@ -19966,7 +20090,7 @@
       <c r="F321" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G321" t="s">
+      <c r="G321" s="10" t="s">
         <v>2526</v>
       </c>
     </row>
@@ -19989,7 +20113,7 @@
       <c r="F322" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G322" t="s">
+      <c r="G322" s="10" t="s">
         <v>2456</v>
       </c>
     </row>
@@ -20010,7 +20134,7 @@
       <c r="F323" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G323" t="s">
+      <c r="G323" s="10" t="s">
         <v>2478</v>
       </c>
     </row>
@@ -20033,7 +20157,7 @@
       <c r="F324" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G324" t="s">
+      <c r="G324" s="10" t="s">
         <v>2479</v>
       </c>
     </row>
@@ -20056,7 +20180,7 @@
       <c r="F325" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G325" t="s">
+      <c r="G325" s="10" t="s">
         <v>2457</v>
       </c>
     </row>
@@ -20079,7 +20203,7 @@
       <c r="F326" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G326" t="s">
+      <c r="G326" s="10" t="s">
         <v>2480</v>
       </c>
     </row>
@@ -20100,7 +20224,7 @@
       <c r="F327" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G327" t="s">
+      <c r="G327" s="10" t="s">
         <v>2481</v>
       </c>
     </row>
@@ -20123,7 +20247,7 @@
       <c r="F328" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G328" t="s">
+      <c r="G328" s="10" t="s">
         <v>2458</v>
       </c>
     </row>
@@ -20146,7 +20270,7 @@
       <c r="F329" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G329" t="s">
+      <c r="G329" s="10" t="s">
         <v>2482</v>
       </c>
     </row>
@@ -20169,7 +20293,7 @@
       <c r="F330" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G330" t="s">
+      <c r="G330" s="10" t="s">
         <v>2459</v>
       </c>
     </row>
@@ -20192,7 +20316,7 @@
       <c r="F331" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G331" t="s">
+      <c r="G331" s="10" t="s">
         <v>2483</v>
       </c>
     </row>
@@ -20215,7 +20339,7 @@
       <c r="F332" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G332" t="s">
+      <c r="G332" s="10" t="s">
         <v>2460</v>
       </c>
     </row>
@@ -20238,7 +20362,7 @@
       <c r="F333" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G333" t="s">
+      <c r="G333" s="10" t="s">
         <v>2461</v>
       </c>
     </row>
@@ -20261,7 +20385,7 @@
       <c r="F334" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G334" t="s">
+      <c r="G334" s="10" t="s">
         <v>2527</v>
       </c>
     </row>
@@ -20284,7 +20408,7 @@
       <c r="F335" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G335" t="s">
+      <c r="G335" s="10" t="s">
         <v>2484</v>
       </c>
     </row>
@@ -20307,7 +20431,7 @@
       <c r="F336" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G336" t="s">
+      <c r="G336" s="10" t="s">
         <v>2464</v>
       </c>
     </row>
@@ -20330,7 +20454,7 @@
       <c r="F337" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G337" t="s">
+      <c r="G337" s="10" t="s">
         <v>2465</v>
       </c>
     </row>
@@ -20351,7 +20475,7 @@
       <c r="F338" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G338" t="s">
+      <c r="G338" s="10" t="s">
         <v>2485</v>
       </c>
     </row>
@@ -20374,7 +20498,7 @@
       <c r="F339" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G339" t="s">
+      <c r="G339" s="10" t="s">
         <v>2528</v>
       </c>
     </row>
@@ -20397,7 +20521,7 @@
       <c r="F340" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G340" t="s">
+      <c r="G340" s="10" t="s">
         <v>2486</v>
       </c>
     </row>
@@ -20420,7 +20544,7 @@
       <c r="F341" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G341" t="s">
+      <c r="G341" s="10" t="s">
         <v>2487</v>
       </c>
     </row>
@@ -20443,7 +20567,7 @@
       <c r="F342" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G342" t="s">
+      <c r="G342" s="10" t="s">
         <v>2488</v>
       </c>
     </row>
@@ -20466,7 +20590,7 @@
       <c r="F343" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G343" t="s">
+      <c r="G343" s="10" t="s">
         <v>2489</v>
       </c>
     </row>
@@ -20487,7 +20611,7 @@
       <c r="F344" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G344" t="s">
+      <c r="G344" s="10" t="s">
         <v>2490</v>
       </c>
     </row>
@@ -20510,7 +20634,7 @@
       <c r="F345" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G345" t="s">
+      <c r="G345" s="10" t="s">
         <v>2491</v>
       </c>
     </row>
@@ -20531,7 +20655,7 @@
       <c r="F346" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G346" t="s">
+      <c r="G346" s="10" t="s">
         <v>2492</v>
       </c>
     </row>
@@ -20554,7 +20678,7 @@
       <c r="F347" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G347" t="s">
+      <c r="G347" s="10" t="s">
         <v>2529</v>
       </c>
     </row>
@@ -20575,7 +20699,7 @@
       <c r="F348" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G348" t="s">
+      <c r="G348" s="10" t="s">
         <v>2493</v>
       </c>
     </row>
@@ -20596,7 +20720,7 @@
       <c r="F349" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G349" t="s">
+      <c r="G349" s="10" t="s">
         <v>2494</v>
       </c>
     </row>
@@ -20617,7 +20741,7 @@
       <c r="F350" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G350" t="s">
+      <c r="G350" s="10" t="s">
         <v>2495</v>
       </c>
     </row>
@@ -20640,7 +20764,7 @@
       <c r="F351" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G351" t="s">
+      <c r="G351" s="10" t="s">
         <v>2530</v>
       </c>
     </row>
@@ -20661,7 +20785,7 @@
       <c r="F352" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G352" t="s">
+      <c r="G352" s="10" t="s">
         <v>2496</v>
       </c>
     </row>
@@ -20684,7 +20808,7 @@
       <c r="F353" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G353" t="s">
+      <c r="G353" s="10" t="s">
         <v>2531</v>
       </c>
     </row>
@@ -20705,7 +20829,7 @@
       <c r="F354" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G354" t="s">
+      <c r="G354" s="10" t="s">
         <v>2497</v>
       </c>
     </row>
@@ -20728,7 +20852,7 @@
       <c r="F355" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G355" t="s">
+      <c r="G355" s="10" t="s">
         <v>2532</v>
       </c>
     </row>
@@ -20751,7 +20875,7 @@
       <c r="F356" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G356" t="s">
+      <c r="G356" s="10" t="s">
         <v>2533</v>
       </c>
     </row>
@@ -20774,7 +20898,7 @@
       <c r="F357" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G357" t="s">
+      <c r="G357" s="10" t="s">
         <v>2498</v>
       </c>
     </row>
@@ -20797,7 +20921,7 @@
       <c r="F358" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G358" t="s">
+      <c r="G358" s="10" t="s">
         <v>2499</v>
       </c>
     </row>
@@ -20820,7 +20944,7 @@
       <c r="F359" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G359" t="s">
+      <c r="G359" s="10" t="s">
         <v>2466</v>
       </c>
     </row>
@@ -20843,7 +20967,7 @@
       <c r="F360" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G360" t="s">
+      <c r="G360" s="10" t="s">
         <v>2534</v>
       </c>
     </row>
@@ -20866,7 +20990,7 @@
       <c r="F361" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G361" t="s">
+      <c r="G361" s="10" t="s">
         <v>2500</v>
       </c>
     </row>
@@ -20889,7 +21013,7 @@
       <c r="F362" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G362" t="s">
+      <c r="G362" s="10" t="s">
         <v>2467</v>
       </c>
     </row>
@@ -20912,7 +21036,7 @@
       <c r="F363" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G363" t="s">
+      <c r="G363" s="10" t="s">
         <v>2501</v>
       </c>
     </row>
@@ -20935,7 +21059,7 @@
       <c r="F364" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G364" t="s">
+      <c r="G364" s="10" t="s">
         <v>2502</v>
       </c>
     </row>
@@ -20958,7 +21082,7 @@
       <c r="F365" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G365" t="s">
+      <c r="G365" s="10" t="s">
         <v>2503</v>
       </c>
     </row>
@@ -20981,7 +21105,7 @@
       <c r="F366" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G366" t="s">
+      <c r="G366" s="10" t="s">
         <v>2504</v>
       </c>
     </row>
@@ -21002,7 +21126,7 @@
       <c r="F367" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G367" t="s">
+      <c r="G367" s="10" t="s">
         <v>2505</v>
       </c>
     </row>
@@ -21023,7 +21147,7 @@
       <c r="F368" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G368" t="s">
+      <c r="G368" s="10" t="s">
         <v>2506</v>
       </c>
     </row>
@@ -21046,7 +21170,7 @@
       <c r="F369" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G369" t="s">
+      <c r="G369" s="10" t="s">
         <v>2507</v>
       </c>
     </row>
@@ -21067,7 +21191,7 @@
       <c r="F370" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G370" t="s">
+      <c r="G370" s="10" t="s">
         <v>2508</v>
       </c>
     </row>
@@ -21090,7 +21214,7 @@
       <c r="F371" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G371" t="s">
+      <c r="G371" s="10" t="s">
         <v>2469</v>
       </c>
     </row>
@@ -21111,7 +21235,7 @@
       <c r="F372" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G372" t="s">
+      <c r="G372" s="10" t="s">
         <v>2509</v>
       </c>
     </row>
@@ -21134,7 +21258,7 @@
       <c r="F373" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G373" t="s">
+      <c r="G373" s="10" t="s">
         <v>2510</v>
       </c>
     </row>
@@ -21157,7 +21281,7 @@
       <c r="F374" s="10" t="s">
         <v>2518</v>
       </c>
-      <c r="G374" t="s">
+      <c r="G374" s="10" t="s">
         <v>2511</v>
       </c>
     </row>
@@ -21180,7 +21304,7 @@
       <c r="F375" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G375" t="s">
+      <c r="G375" s="10" t="s">
         <v>2471</v>
       </c>
     </row>
@@ -21201,8 +21325,376 @@
       <c r="F376" s="10" t="s">
         <v>2519</v>
       </c>
-      <c r="G376" t="s">
+      <c r="G376" s="10" t="s">
         <v>2512</v>
+      </c>
+    </row>
+    <row r="377" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A377">
+        <v>376</v>
+      </c>
+      <c r="B377" t="s">
+        <v>2536</v>
+      </c>
+      <c r="C377" t="s">
+        <v>2547</v>
+      </c>
+      <c r="D377" t="s">
+        <v>2</v>
+      </c>
+      <c r="E377" s="10">
+        <v>3</v>
+      </c>
+      <c r="F377" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="G377" s="10" t="s">
+        <v>2567</v>
+      </c>
+    </row>
+    <row r="378" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A378">
+        <v>377</v>
+      </c>
+      <c r="B378" t="s">
+        <v>2537</v>
+      </c>
+      <c r="C378" t="s">
+        <v>2547</v>
+      </c>
+      <c r="D378" t="s">
+        <v>2</v>
+      </c>
+      <c r="E378" s="10">
+        <v>3</v>
+      </c>
+      <c r="F378" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="G378" s="10" t="s">
+        <v>2563</v>
+      </c>
+    </row>
+    <row r="379" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A379">
+        <v>378</v>
+      </c>
+      <c r="B379" t="s">
+        <v>2538</v>
+      </c>
+      <c r="C379" t="s">
+        <v>2547</v>
+      </c>
+      <c r="D379" t="s">
+        <v>2</v>
+      </c>
+      <c r="E379" s="10">
+        <v>3</v>
+      </c>
+      <c r="F379" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="G379" s="10" t="s">
+        <v>2539</v>
+      </c>
+    </row>
+    <row r="380" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A380">
+        <v>379</v>
+      </c>
+      <c r="B380" t="s">
+        <v>2540</v>
+      </c>
+      <c r="C380" t="s">
+        <v>2547</v>
+      </c>
+      <c r="D380" t="s">
+        <v>2</v>
+      </c>
+      <c r="E380" s="10">
+        <v>6</v>
+      </c>
+      <c r="F380" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="G380" s="10" t="s">
+        <v>2568</v>
+      </c>
+    </row>
+    <row r="381" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A381">
+        <v>380</v>
+      </c>
+      <c r="B381" t="s">
+        <v>2541</v>
+      </c>
+      <c r="C381" t="s">
+        <v>2547</v>
+      </c>
+      <c r="D381" t="s">
+        <v>2</v>
+      </c>
+      <c r="E381" s="10">
+        <v>5</v>
+      </c>
+      <c r="F381" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="G381" s="10" t="s">
+        <v>2564</v>
+      </c>
+    </row>
+    <row r="382" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A382">
+        <v>381</v>
+      </c>
+      <c r="B382" t="s">
+        <v>2543</v>
+      </c>
+      <c r="C382" t="s">
+        <v>2547</v>
+      </c>
+      <c r="D382" t="s">
+        <v>2</v>
+      </c>
+      <c r="E382" s="10">
+        <v>4</v>
+      </c>
+      <c r="F382" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="G382" s="10" t="s">
+        <v>2569</v>
+      </c>
+    </row>
+    <row r="383" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A383">
+        <v>382</v>
+      </c>
+      <c r="B383" t="s">
+        <v>2545</v>
+      </c>
+      <c r="C383" t="s">
+        <v>2547</v>
+      </c>
+      <c r="D383" t="s">
+        <v>18</v>
+      </c>
+      <c r="E383" s="10">
+        <v>5</v>
+      </c>
+      <c r="F383" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="G383" s="10" t="s">
+        <v>2546</v>
+      </c>
+    </row>
+    <row r="384" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A384">
+        <v>383</v>
+      </c>
+      <c r="B384" t="s">
+        <v>2548</v>
+      </c>
+      <c r="C384" t="s">
+        <v>2562</v>
+      </c>
+      <c r="D384" t="s">
+        <v>2</v>
+      </c>
+      <c r="E384" s="10">
+        <v>2</v>
+      </c>
+      <c r="F384" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="G384" s="10" t="s">
+        <v>2565</v>
+      </c>
+    </row>
+    <row r="385" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A385">
+        <v>384</v>
+      </c>
+      <c r="B385" t="s">
+        <v>2550</v>
+      </c>
+      <c r="C385" t="s">
+        <v>2562</v>
+      </c>
+      <c r="D385" t="s">
+        <v>63</v>
+      </c>
+      <c r="E385" s="10">
+        <v>4</v>
+      </c>
+      <c r="F385" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="G385" s="10" t="s">
+        <v>2570</v>
+      </c>
+    </row>
+    <row r="386" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A386">
+        <v>385</v>
+      </c>
+      <c r="B386" t="s">
+        <v>2552</v>
+      </c>
+      <c r="C386" t="s">
+        <v>2562</v>
+      </c>
+      <c r="D386" t="s">
+        <v>7</v>
+      </c>
+      <c r="E386" s="10">
+        <v>4</v>
+      </c>
+      <c r="F386" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="G386" s="10" t="s">
+        <v>2553</v>
+      </c>
+    </row>
+    <row r="387" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A387">
+        <v>386</v>
+      </c>
+      <c r="B387" t="s">
+        <v>2555</v>
+      </c>
+      <c r="C387" t="s">
+        <v>2562</v>
+      </c>
+      <c r="D387" t="s">
+        <v>2</v>
+      </c>
+      <c r="E387" s="10">
+        <v>5</v>
+      </c>
+      <c r="F387" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="G387" s="10" t="s">
+        <v>2556</v>
+      </c>
+    </row>
+    <row r="388" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A388">
+        <v>387</v>
+      </c>
+      <c r="B388" t="s">
+        <v>2557</v>
+      </c>
+      <c r="C388" t="s">
+        <v>2562</v>
+      </c>
+      <c r="D388" t="s">
+        <v>18</v>
+      </c>
+      <c r="E388" s="10">
+        <v>5</v>
+      </c>
+      <c r="F388" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="G388" s="10" t="s">
+        <v>2571</v>
+      </c>
+    </row>
+    <row r="389" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A389">
+        <v>388</v>
+      </c>
+      <c r="B389" t="s">
+        <v>2558</v>
+      </c>
+      <c r="C389" t="s">
+        <v>2562</v>
+      </c>
+      <c r="D389" t="s">
+        <v>2</v>
+      </c>
+      <c r="E389" s="10">
+        <v>4</v>
+      </c>
+      <c r="F389" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="G389" s="10" t="s">
+        <v>2566</v>
+      </c>
+    </row>
+    <row r="390" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A390">
+        <v>389</v>
+      </c>
+      <c r="B390" t="s">
+        <v>2560</v>
+      </c>
+      <c r="C390" t="s">
+        <v>2562</v>
+      </c>
+      <c r="D390" t="s">
+        <v>2</v>
+      </c>
+      <c r="E390" s="10">
+        <v>5</v>
+      </c>
+      <c r="F390" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="G390" s="10" t="s">
+        <v>2572</v>
+      </c>
+    </row>
+    <row r="391" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A391">
+        <v>390</v>
+      </c>
+      <c r="B391" t="s">
+        <v>2573</v>
+      </c>
+      <c r="C391" t="s">
+        <v>344</v>
+      </c>
+      <c r="D391" t="s">
+        <v>2</v>
+      </c>
+      <c r="E391" s="10" t="s">
+        <v>2156</v>
+      </c>
+      <c r="F391" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="G391" s="10" t="s">
+        <v>2574</v>
+      </c>
+    </row>
+    <row r="392" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A392">
+        <v>391</v>
+      </c>
+      <c r="B392" t="s">
+        <v>2576</v>
+      </c>
+      <c r="C392" t="s">
+        <v>344</v>
+      </c>
+      <c r="D392" t="s">
+        <v>2</v>
+      </c>
+      <c r="E392" s="10" t="s">
+        <v>601</v>
+      </c>
+      <c r="F392" s="10" t="s">
+        <v>2519</v>
+      </c>
+      <c r="G392" s="5" t="s">
+        <v>2575</v>
       </c>
     </row>
   </sheetData>
@@ -21216,6 +21708,412 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="A1:F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="6" max="6" width="124.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2536</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2547</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>2567</v>
+      </c>
+      <c r="G1">
+        <v>1</v>
+      </c>
+      <c r="H1">
+        <v>1</v>
+      </c>
+      <c r="J1" t="e">
+        <f>+Coin1.png?</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2537</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2547</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>2563</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2538</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2547</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>2539</v>
+      </c>
+      <c r="J3" t="e">
+        <f>+Coin2.png</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2540</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2547</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>2568</v>
+      </c>
+      <c r="G4">
+        <v>-1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2541</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2547</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>2564</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>2542</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2543</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2547</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>2569</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2544</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="J6" t="e">
+        <f>+Coin1</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2545</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2547</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>2546</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2548</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2562</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>2565</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="K8" t="s">
+        <v>2549</v>
+      </c>
+      <c r="M8" t="s">
+        <v>2549</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2550</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2562</v>
+      </c>
+      <c r="C9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>2570</v>
+      </c>
+      <c r="G9" t="s">
+        <v>2551</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="J9" t="e">
+        <f>+Coin2?</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2552</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2562</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>2553</v>
+      </c>
+      <c r="G10" t="s">
+        <v>2554</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2555</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2562</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>2556</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2557</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2562</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>2571</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12" t="s">
+        <v>2549</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2558</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2562</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>2566</v>
+      </c>
+      <c r="G13" t="s">
+        <v>2559</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2560</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2562</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>2518</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>2572</v>
+      </c>
+      <c r="H14" t="s">
+        <v>2561</v>
+      </c>
+      <c r="I14" t="s">
+        <v>2561</v>
+      </c>
+      <c r="J14" t="e">
+        <f>+Coin3.png?</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M14" t="s">
+        <v>2549</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21555,7 +22453,7 @@
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>195</v>
       </c>
@@ -21657,7 +22555,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>289</v>
       </c>

</xml_diff>